<commit_message>
5 excel files updated
</commit_message>
<xml_diff>
--- a/ExcelFiles/April_Quotey_Gold_202104.xlsx
+++ b/ExcelFiles/April_Quotey_Gold_202104.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/345d1610474a9baa/Quotey McQuoteface/Rating and Covermatch/Rating 20020723/Contractors/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="8_{87AD32E3-AA58-470B-87B3-9F8C33176638}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{83F30469-33F2-4420-9179-FC7041CF5FF4}"/>
+  <xr:revisionPtr revIDLastSave="57" documentId="8_{87AD32E3-AA58-470B-87B3-9F8C33176638}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{12385A35-CEFB-4A81-B728-66F5C0CBDF93}"/>
   <workbookProtection workbookPassword="93C0" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-4110" windowWidth="29040" windowHeight="15840" tabRatio="444" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -4282,7 +4282,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="61">
+  <fills count="62">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4622,6 +4622,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF66CC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -10039,7 +10045,7 @@
     <xf numFmtId="0" fontId="41" fillId="55" borderId="60" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="41" fillId="55" borderId="60" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="625">
+  <cellXfs count="634">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="17" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="17" fillId="27" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -11354,6 +11360,21 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="42" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="42" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="4" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -11396,6 +11417,42 @@
     <xf numFmtId="0" fontId="0" fillId="31" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="0" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="0" borderId="72" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="0" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="0" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="65" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="66" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="0" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="168" fontId="58" fillId="0" borderId="74" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -11405,12 +11462,6 @@
     <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="58" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="58" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="59" fillId="56" borderId="61" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -11426,9 +11477,6 @@
     <xf numFmtId="10" fontId="58" fillId="0" borderId="71" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="58" fillId="0" borderId="72" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="58" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -11444,33 +11492,6 @@
     <xf numFmtId="9" fontId="58" fillId="0" borderId="65" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="58" fillId="0" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="58" fillId="0" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="58" fillId="0" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="65" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="66" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="58" fillId="0" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="58" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="58" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="168" fontId="19" fillId="0" borderId="39" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -11537,24 +11558,40 @@
     <xf numFmtId="0" fontId="19" fillId="42" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="4" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="25" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="25" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="19" fillId="34" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="19" fillId="34" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="19" fillId="34" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="19" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="61" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="19" fillId="34" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4345">
     <cellStyle name="20 % - Accent1 2" xfId="7" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -16816,7 +16853,7 @@
   <dimension ref="A1:AT264"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelCol="1"/>
@@ -16906,23 +16943,23 @@
     </row>
     <row r="2" spans="1:37" s="20" customFormat="1" ht="30.75" customHeight="1" thickBot="1">
       <c r="A2" s="17"/>
-      <c r="B2" s="561" t="s">
+      <c r="B2" s="566" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="562"/>
-      <c r="D2" s="563" t="s">
+      <c r="C2" s="567"/>
+      <c r="D2" s="568" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="564"/>
-      <c r="F2" s="564"/>
-      <c r="G2" s="564"/>
-      <c r="H2" s="564"/>
-      <c r="I2" s="564"/>
-      <c r="J2" s="564"/>
-      <c r="K2" s="564"/>
-      <c r="L2" s="564"/>
-      <c r="M2" s="564"/>
-      <c r="N2" s="564"/>
+      <c r="E2" s="569"/>
+      <c r="F2" s="569"/>
+      <c r="G2" s="569"/>
+      <c r="H2" s="569"/>
+      <c r="I2" s="569"/>
+      <c r="J2" s="569"/>
+      <c r="K2" s="569"/>
+      <c r="L2" s="569"/>
+      <c r="M2" s="569"/>
+      <c r="N2" s="569"/>
       <c r="O2" s="18" t="s">
         <v>8</v>
       </c>
@@ -16939,21 +16976,21 @@
       <c r="Z2" s="19"/>
       <c r="AA2" s="19"/>
       <c r="AB2" s="19"/>
-      <c r="AC2" s="565" t="s">
+      <c r="AC2" s="570" t="s">
         <v>9</v>
       </c>
-      <c r="AD2" s="566"/>
-      <c r="AE2" s="567" t="s">
+      <c r="AD2" s="571"/>
+      <c r="AE2" s="572" t="s">
         <v>10</v>
       </c>
-      <c r="AF2" s="568"/>
-      <c r="AG2" s="569"/>
-      <c r="AH2" s="556" t="s">
+      <c r="AF2" s="573"/>
+      <c r="AG2" s="574"/>
+      <c r="AH2" s="561" t="s">
         <v>11</v>
       </c>
-      <c r="AI2" s="557"/>
-      <c r="AJ2" s="557"/>
-      <c r="AK2" s="558"/>
+      <c r="AI2" s="562"/>
+      <c r="AJ2" s="562"/>
+      <c r="AK2" s="563"/>
     </row>
     <row r="4" spans="1:37">
       <c r="E4" s="23" t="s">
@@ -16996,15 +17033,15 @@
       <c r="H5" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="I5" s="559" t="str">
+      <c r="I5" s="564" t="str">
         <f>IF($M$9&lt;&gt;"",$M$9,IF($M$10&lt;&gt;"",$M$10,IF($M$11&lt;&gt;"",$M$11,IF($M$12&lt;&gt;"",$M$12,IF($M$13&lt;&gt;"",$M$13,IF($M$14&lt;&gt;"",$M$14,IF($M$15&lt;&gt;"",$M$15,IF($M$16&lt;&gt;"",$M$16,IF($M$17&lt;&gt;"",$M$17,IF($M$18&lt;&gt;"",$M$18,IF($M$24&lt;&gt;"",$M$24,IF($M$25&lt;&gt;"",$M$25,IF($M$26&lt;&gt;"",$M$26,IF($M$27&lt;&gt;"",$M$27,IF($M$28&lt;&gt;"",$M$28,IF($M$29&lt;&gt;"",$M$29,IF($M$30&lt;&gt;"",$M$30,IF($M$31&lt;&gt;"",$M$31,IF($M$32&lt;&gt;"",$M$32,IF($M$33&lt;&gt;"",$M$33,IF($M$19&lt;&gt;"",$M$19,IF($M$20&lt;&gt;"",$M$20,IF($M$21&lt;&gt;"",$M$21,IF($M$22&lt;&gt;"",$M$22,IF($M$23&lt;&gt;"",$M$23,IF($M$38&lt;&gt;"",$M$38,IF($M$39&lt;&gt;"",$M$39,IF($M$40&lt;&gt;"",$M$40,IF($M$41&lt;&gt;"",$M$41,IF($M$42&lt;&gt;"",$M$42,IF($M$43&lt;&gt;"",$M$43,IF($M$44&lt;&gt;"",$M$44,IF($M$45&lt;&gt;"",$M$45,IF($M$46&lt;&gt;"",$M$46,IF($M$47&lt;&gt;"",$M$47,IF($M$48&lt;&gt;"",$M$48,IF($M$49&lt;&gt;"",$M$49,IF($M$50&lt;&gt;"",$M$50,IF($M$51&lt;&gt;"",$M$51,IF($M$52&lt;&gt;"",$M$52,IF($M$53&lt;&gt;"",$M$53,IF($M$54&lt;&gt;"",$M$54,IF($M$55&lt;&gt;"",$M$55,IF($M$56&lt;&gt;"",$M$56,IF($M$57&lt;&gt;"",$M$57,IF($M$58&lt;&gt;"",$M$58,IF($M$59&lt;&gt;"",$M$59,IF($M$60&lt;&gt;"",$M$60,IF($M$61&lt;&gt;"",$M$61,IF($M$62&lt;&gt;"",$M$62,IF($M$63&lt;&gt;"",$M$63,IF($M$64&lt;&gt;"",$M$64,IF($M$65&lt;&gt;"",$M$65,IF($M$66&lt;&gt;"",$M$66,IF($M$67&lt;&gt;"",$M$67,IF($M$68&lt;&gt;"",$M$68,IF($M$69&lt;&gt;"",$M$69,IF($M$70&lt;&gt;"",$M$70,IF($M$71&lt;&gt;"",$M$71,IF($M$72&lt;&gt;"",$M$72,IF($M$73&lt;&gt;"",$M$73,IF($M$74&lt;&gt;"",$M$74,IF($M$75&lt;&gt;"",$M$75,IF($M$76&lt;&gt;"",$M$76,""))))))))))))))))))))))))))))))))))))))))))))))))))))))))))))))))</f>
         <v>Previous claims</v>
       </c>
-      <c r="J5" s="559"/>
-      <c r="K5" s="559"/>
-      <c r="L5" s="559"/>
-      <c r="M5" s="559"/>
-      <c r="N5" s="559"/>
+      <c r="J5" s="564"/>
+      <c r="K5" s="564"/>
+      <c r="L5" s="564"/>
+      <c r="M5" s="564"/>
+      <c r="N5" s="564"/>
       <c r="O5" s="35" t="s">
         <v>19</v>
       </c>
@@ -17044,13 +17081,13 @@
       </c>
     </row>
     <row r="6" spans="1:37" ht="15" thickTop="1">
-      <c r="A6" s="618" t="s">
+      <c r="A6" s="556" t="s">
         <v>1131</v>
       </c>
       <c r="B6" s="41" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="617"/>
+      <c r="C6" s="622"/>
       <c r="E6" t="s">
         <v>29</v>
       </c>
@@ -17061,15 +17098,15 @@
       <c r="H6" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="I6" s="559" t="e">
+      <c r="I6" s="564" t="e">
         <f>IF($N$9&lt;&gt;"",$N$9,IF($N$10&lt;&gt;"",$N$10,IF($N$11&lt;&gt;"",$N$11,IF($N$12&lt;&gt;"",$N$12,IF($N$13&lt;&gt;"",$N$13,IF($N$14&lt;&gt;"",$N$14,IF($N$15&lt;&gt;"",$N$15,IF($N$16&lt;&gt;"",$N$16,IF($N$17&lt;&gt;"",$N$17,IF($N$18&lt;&gt;"",$N$18,IF($N$24&lt;&gt;"",$N$24,IF($N$25&lt;&gt;"",$N$25,IF($N$26&lt;&gt;"",$N$26,IF($N$27&lt;&gt;"",$N$27,IF($N$28&lt;&gt;"",$N$28,IF($N$29&lt;&gt;"",$N$29,IF($N$30&lt;&gt;"",$N$30,IF($N$31&lt;&gt;"",$N$31,IF($N$32&lt;&gt;"",$N$32,IF($N$33&lt;&gt;"",$N$33,IF($N$19&lt;&gt;"",$N$19,IF($N$20&lt;&gt;"",$N$20,IF($N$21&lt;&gt;"",$N$21,IF($N$22&lt;&gt;"",$N$22,IF($N$23&lt;&gt;"",$N$23,IF($N$38&lt;&gt;"",$N$38,IF($N$39&lt;&gt;"",$N$39,IF($N$40&lt;&gt;"",$N$40,IF($N$41&lt;&gt;"",$N$41,IF($N$42&lt;&gt;"",$N$42,IF($N$43&lt;&gt;"",$N$43,IF($N$44&lt;&gt;"",$N$44,IF($N$45&lt;&gt;"",$N$45,IF($N$46&lt;&gt;"",$N$46,IF($N$47&lt;&gt;"",$N$47,IF($N$48&lt;&gt;"",$N$48,IF($N$49&lt;&gt;"",$N$49,IF($N$50&lt;&gt;"",$N$50,IF($N$51&lt;&gt;"",$N$51,IF($N$52&lt;&gt;"",$N$52,IF($N$53&lt;&gt;"",$N$53,IF($N$54&lt;&gt;"",$N$54,IF($N$55&lt;&gt;"",$N$55,IF($N$56&lt;&gt;"",$N$56,IF($N$57&lt;&gt;"",$N$57,IF($N$58&lt;&gt;"",$N$58,IF($N$59&lt;&gt;"",$N$59,IF($N$60&lt;&gt;"",$N$60,IF($N$61&lt;&gt;"",$N$61,IF($N$62&lt;&gt;"",$N$62,IF($N$63&lt;&gt;"",$N$63,IF($N$64&lt;&gt;"",$N$64,IF($N$65&lt;&gt;"",$N$65,IF($N$66&lt;&gt;"",$N$66,IF($N$67&lt;&gt;"",$N$67,IF($N$68&lt;&gt;"",$N$68,IF($N$69&lt;&gt;"",$N$69,IF($N$70&lt;&gt;"",$N$70,IF($N$71&lt;&gt;"",$N$71,IF($N$72&lt;&gt;"",$N$72,IF($N$73&lt;&gt;"",$N$73,IF($N$74&lt;&gt;"",$N$74,IF($N$75&lt;&gt;"",$N$75,IF($N$76&lt;&gt;"",$N$76,""))))))))))))))))))))))))))))))))))))))))))))))))))))))))))))))))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="J6" s="559"/>
-      <c r="K6" s="559"/>
-      <c r="L6" s="559"/>
-      <c r="M6" s="559"/>
-      <c r="N6" s="559"/>
+      <c r="J6" s="564"/>
+      <c r="K6" s="564"/>
+      <c r="L6" s="564"/>
+      <c r="M6" s="564"/>
+      <c r="N6" s="564"/>
       <c r="O6" s="22">
         <v>175200</v>
       </c>
@@ -17098,13 +17135,13 @@
       </c>
     </row>
     <row r="7" spans="1:37">
-      <c r="A7" s="618">
+      <c r="A7" s="556">
         <v>650000</v>
       </c>
       <c r="B7" s="45" t="s">
         <v>36</v>
       </c>
-      <c r="C7" s="47"/>
+      <c r="C7" s="623"/>
       <c r="E7" s="23"/>
       <c r="F7" s="23"/>
       <c r="G7" s="26"/>
@@ -17152,17 +17189,17 @@
       </c>
     </row>
     <row r="8" spans="1:37" ht="29.4" thickBot="1">
-      <c r="A8" s="618">
+      <c r="A8" s="556">
         <v>650100</v>
       </c>
       <c r="B8" s="45" t="s">
         <v>40</v>
       </c>
-      <c r="C8" s="76"/>
-      <c r="D8" s="560" t="s">
+      <c r="C8" s="623"/>
+      <c r="D8" s="565" t="s">
         <v>41</v>
       </c>
-      <c r="E8" s="560"/>
+      <c r="E8" s="565"/>
       <c r="F8" s="49" t="s">
         <v>42</v>
       </c>
@@ -17231,14 +17268,14 @@
       </c>
     </row>
     <row r="9" spans="1:37">
-      <c r="A9" s="619">
+      <c r="A9" s="557">
         <v>510</v>
       </c>
       <c r="B9" s="45" t="s">
         <v>54</v>
       </c>
-      <c r="C9" s="76"/>
-      <c r="D9" s="620">
+      <c r="C9" s="624"/>
+      <c r="D9" s="558">
         <v>1</v>
       </c>
       <c r="E9" s="54" t="s">
@@ -17315,13 +17352,13 @@
       </c>
     </row>
     <row r="10" spans="1:37">
-      <c r="A10" s="619">
+      <c r="A10" s="557">
         <v>513</v>
       </c>
       <c r="B10" s="45" t="s">
         <v>63</v>
       </c>
-      <c r="C10" s="76"/>
+      <c r="C10" s="623"/>
       <c r="D10" s="545">
         <v>2</v>
       </c>
@@ -17401,13 +17438,13 @@
       </c>
     </row>
     <row r="11" spans="1:37">
-      <c r="A11" s="619">
+      <c r="A11" s="557">
         <v>10508</v>
       </c>
       <c r="B11" s="45" t="s">
         <v>70</v>
       </c>
-      <c r="C11" s="76"/>
+      <c r="C11" s="623"/>
       <c r="D11" s="545">
         <v>3</v>
       </c>
@@ -17487,13 +17524,13 @@
       </c>
     </row>
     <row r="12" spans="1:37">
-      <c r="A12" s="619">
+      <c r="A12" s="557">
         <v>519</v>
       </c>
       <c r="B12" s="45" t="s">
         <v>79</v>
       </c>
-      <c r="C12" s="76"/>
+      <c r="C12" s="623"/>
       <c r="D12" s="545">
         <v>4</v>
       </c>
@@ -17574,13 +17611,13 @@
       </c>
     </row>
     <row r="13" spans="1:37">
-      <c r="A13" s="619">
+      <c r="A13" s="557">
         <v>523</v>
       </c>
       <c r="B13" s="45" t="s">
         <v>87</v>
       </c>
-      <c r="C13" s="76"/>
+      <c r="C13" s="625"/>
       <c r="D13" s="545">
         <v>5</v>
       </c>
@@ -17661,13 +17698,13 @@
       <c r="AK13" s="63"/>
     </row>
     <row r="14" spans="1:37">
-      <c r="A14" s="619">
+      <c r="A14" s="557">
         <v>650500</v>
       </c>
       <c r="B14" s="45" t="s">
         <v>96</v>
       </c>
-      <c r="C14" s="76"/>
+      <c r="C14" s="623"/>
       <c r="D14" s="545">
         <v>6</v>
       </c>
@@ -17747,13 +17784,13 @@
       </c>
     </row>
     <row r="15" spans="1:37">
-      <c r="A15" s="619">
+      <c r="A15" s="557">
         <v>527</v>
       </c>
       <c r="B15" s="45" t="s">
         <v>105</v>
       </c>
-      <c r="C15" s="76"/>
+      <c r="C15" s="626"/>
       <c r="D15" s="545">
         <v>7</v>
       </c>
@@ -17831,13 +17868,13 @@
       </c>
     </row>
     <row r="16" spans="1:37">
-      <c r="A16" s="619">
+      <c r="A16" s="557">
         <v>529</v>
       </c>
       <c r="B16" s="47" t="s">
         <v>1110</v>
       </c>
-      <c r="C16" s="76"/>
+      <c r="C16" s="626"/>
       <c r="D16" s="545">
         <v>8</v>
       </c>
@@ -17915,13 +17952,13 @@
       </c>
     </row>
     <row r="17" spans="1:46">
-      <c r="A17" s="619">
+      <c r="A17" s="557">
         <v>538</v>
       </c>
       <c r="B17" s="47" t="s">
         <v>1111</v>
       </c>
-      <c r="C17" s="76"/>
+      <c r="C17" s="626"/>
       <c r="D17" s="545">
         <v>9</v>
       </c>
@@ -18001,13 +18038,13 @@
       </c>
     </row>
     <row r="18" spans="1:46">
-      <c r="A18" s="618" t="s">
+      <c r="A18" s="556" t="s">
         <v>113</v>
       </c>
       <c r="B18" s="47" t="s">
         <v>114</v>
       </c>
-      <c r="C18" s="76"/>
+      <c r="C18" s="627"/>
       <c r="D18" s="545">
         <v>10</v>
       </c>
@@ -18087,13 +18124,13 @@
       </c>
     </row>
     <row r="19" spans="1:46">
-      <c r="A19" s="618" t="s">
+      <c r="A19" s="556" t="s">
         <v>1132</v>
       </c>
       <c r="B19" s="65" t="s">
         <v>122</v>
       </c>
-      <c r="C19" s="623"/>
+      <c r="C19" s="628"/>
       <c r="D19" s="545">
         <v>11</v>
       </c>
@@ -18171,13 +18208,13 @@
       </c>
     </row>
     <row r="20" spans="1:46">
-      <c r="A20" s="618" t="s">
+      <c r="A20" s="556" t="s">
         <v>1133</v>
       </c>
       <c r="B20" s="65" t="s">
         <v>132</v>
       </c>
-      <c r="C20" s="623"/>
+      <c r="C20" s="629"/>
       <c r="D20" s="545">
         <v>12</v>
       </c>
@@ -18257,13 +18294,13 @@
       </c>
     </row>
     <row r="21" spans="1:46">
-      <c r="A21" s="618" t="s">
+      <c r="A21" s="556" t="s">
         <v>1134</v>
       </c>
       <c r="B21" s="65" t="s">
         <v>141</v>
       </c>
-      <c r="C21" s="623"/>
+      <c r="C21" s="630"/>
       <c r="D21" s="545">
         <v>13</v>
       </c>
@@ -18343,13 +18380,13 @@
       </c>
     </row>
     <row r="22" spans="1:46">
-      <c r="A22" s="618" t="s">
+      <c r="A22" s="556" t="s">
         <v>1135</v>
       </c>
       <c r="B22" s="65" t="s">
         <v>149</v>
       </c>
-      <c r="C22" s="623"/>
+      <c r="C22" s="630"/>
       <c r="D22" s="545">
         <v>14</v>
       </c>
@@ -18429,13 +18466,13 @@
       </c>
     </row>
     <row r="23" spans="1:46">
-      <c r="A23" s="618" t="s">
+      <c r="A23" s="556" t="s">
         <v>1136</v>
       </c>
       <c r="B23" s="65" t="s">
         <v>158</v>
       </c>
-      <c r="C23" s="623"/>
+      <c r="C23" s="630"/>
       <c r="D23" s="545">
         <v>15</v>
       </c>
@@ -18514,13 +18551,13 @@
       </c>
     </row>
     <row r="24" spans="1:46">
-      <c r="A24" s="618" t="s">
+      <c r="A24" s="556" t="s">
         <v>1137</v>
       </c>
       <c r="B24" s="65" t="s">
         <v>166</v>
       </c>
-      <c r="C24" s="623"/>
+      <c r="C24" s="626"/>
       <c r="D24" s="545">
         <v>16</v>
       </c>
@@ -18601,13 +18638,13 @@
       </c>
     </row>
     <row r="25" spans="1:46">
-      <c r="A25" s="618" t="s">
+      <c r="A25" s="556" t="s">
         <v>174</v>
       </c>
       <c r="B25" s="47" t="s">
         <v>175</v>
       </c>
-      <c r="C25" s="76"/>
+      <c r="C25" s="626"/>
       <c r="D25" s="545">
         <v>17</v>
       </c>
@@ -18687,13 +18724,13 @@
       </c>
     </row>
     <row r="26" spans="1:46">
-      <c r="A26" s="618" t="s">
+      <c r="A26" s="556" t="s">
         <v>1138</v>
       </c>
       <c r="B26" s="65" t="s">
         <v>185</v>
       </c>
-      <c r="C26" s="623"/>
+      <c r="C26" s="541"/>
       <c r="D26" s="545">
         <v>18</v>
       </c>
@@ -18773,13 +18810,13 @@
       </c>
     </row>
     <row r="27" spans="1:46">
-      <c r="A27" s="618" t="s">
+      <c r="A27" s="556" t="s">
         <v>1139</v>
       </c>
       <c r="B27" s="65" t="s">
         <v>194</v>
       </c>
-      <c r="C27" s="623"/>
+      <c r="C27" s="630"/>
       <c r="D27" s="545">
         <v>19</v>
       </c>
@@ -18859,13 +18896,13 @@
       </c>
     </row>
     <row r="28" spans="1:46">
-      <c r="A28" s="618" t="s">
+      <c r="A28" s="556" t="s">
         <v>1140</v>
       </c>
       <c r="B28" s="65" t="s">
         <v>203</v>
       </c>
-      <c r="C28" s="623"/>
+      <c r="C28" s="630"/>
       <c r="D28" s="545">
         <v>20</v>
       </c>
@@ -18938,13 +18975,13 @@
       </c>
     </row>
     <row r="29" spans="1:46">
-      <c r="A29" s="618" t="s">
+      <c r="A29" s="556" t="s">
         <v>1141</v>
       </c>
       <c r="B29" s="65" t="s">
         <v>211</v>
       </c>
-      <c r="C29" s="623"/>
+      <c r="C29" s="630"/>
       <c r="D29" s="545">
         <v>21</v>
       </c>
@@ -19017,13 +19054,13 @@
       </c>
     </row>
     <row r="30" spans="1:46">
-      <c r="A30" s="618" t="s">
+      <c r="A30" s="556" t="s">
         <v>1142</v>
       </c>
       <c r="B30" s="65" t="s">
         <v>218</v>
       </c>
-      <c r="C30" s="623"/>
+      <c r="C30" s="630"/>
       <c r="D30" s="545">
         <v>22</v>
       </c>
@@ -19100,13 +19137,13 @@
       </c>
     </row>
     <row r="31" spans="1:46">
-      <c r="A31" s="618" t="s">
+      <c r="A31" s="556" t="s">
         <v>1143</v>
       </c>
       <c r="B31" s="65" t="s">
         <v>222</v>
       </c>
-      <c r="C31" s="623"/>
+      <c r="C31" s="626"/>
       <c r="D31" s="545">
         <v>23</v>
       </c>
@@ -19187,13 +19224,13 @@
       <c r="AT31" s="332"/>
     </row>
     <row r="32" spans="1:46">
-      <c r="A32" s="618" t="s">
+      <c r="A32" s="556" t="s">
         <v>226</v>
       </c>
       <c r="B32" s="47" t="s">
         <v>227</v>
       </c>
-      <c r="C32" s="76"/>
+      <c r="C32" s="626"/>
       <c r="D32" s="545">
         <v>24</v>
       </c>
@@ -19274,13 +19311,13 @@
       <c r="AT32" s="332"/>
     </row>
     <row r="33" spans="1:46">
-      <c r="A33" s="618" t="s">
+      <c r="A33" s="556" t="s">
         <v>1144</v>
       </c>
       <c r="B33" s="65" t="s">
         <v>231</v>
       </c>
-      <c r="C33" s="623"/>
+      <c r="C33" s="541"/>
       <c r="D33" s="545">
         <v>25</v>
       </c>
@@ -19355,13 +19392,13 @@
       <c r="AT33" s="332"/>
     </row>
     <row r="34" spans="1:46">
-      <c r="A34" s="618" t="s">
+      <c r="A34" s="556" t="s">
         <v>1145</v>
       </c>
       <c r="B34" s="65" t="s">
         <v>235</v>
       </c>
-      <c r="C34" s="623"/>
+      <c r="C34" s="630"/>
       <c r="D34" s="545"/>
       <c r="E34" s="47"/>
       <c r="F34" s="47"/>
@@ -19415,13 +19452,13 @@
       <c r="AT34" s="332"/>
     </row>
     <row r="35" spans="1:46">
-      <c r="A35" s="618" t="s">
+      <c r="A35" s="556" t="s">
         <v>1146</v>
       </c>
       <c r="B35" s="65" t="s">
         <v>239</v>
       </c>
-      <c r="C35" s="623"/>
+      <c r="C35" s="630"/>
       <c r="D35" s="545"/>
       <c r="E35" s="47"/>
       <c r="F35" s="47"/>
@@ -19475,14 +19512,14 @@
       <c r="AT35" s="332"/>
     </row>
     <row r="36" spans="1:46">
-      <c r="A36" s="618" t="s">
+      <c r="A36" s="556" t="s">
         <v>1147</v>
       </c>
       <c r="B36" s="65" t="s">
         <v>243</v>
       </c>
-      <c r="C36" s="623"/>
-      <c r="D36" s="621" t="s">
+      <c r="C36" s="630"/>
+      <c r="D36" s="559" t="s">
         <v>1070</v>
       </c>
       <c r="E36" s="47"/>
@@ -19537,13 +19574,13 @@
       <c r="AT36" s="332"/>
     </row>
     <row r="37" spans="1:46" ht="29.4" thickBot="1">
-      <c r="A37" s="618" t="s">
+      <c r="A37" s="556" t="s">
         <v>1148</v>
       </c>
       <c r="B37" s="65" t="s">
         <v>247</v>
       </c>
-      <c r="C37" s="623"/>
+      <c r="C37" s="630"/>
       <c r="D37" s="51"/>
       <c r="E37" s="433" t="s">
         <v>1072</v>
@@ -19617,13 +19654,13 @@
       <c r="AT37" s="332"/>
     </row>
     <row r="38" spans="1:46">
-      <c r="A38" s="618" t="s">
+      <c r="A38" s="556" t="s">
         <v>1149</v>
       </c>
       <c r="B38" s="65" t="s">
         <v>252</v>
       </c>
-      <c r="C38" s="623"/>
+      <c r="C38" s="626"/>
       <c r="D38" s="545"/>
       <c r="E38" s="545">
         <v>175200</v>
@@ -19700,13 +19737,13 @@
       <c r="AT38" s="332"/>
     </row>
     <row r="39" spans="1:46">
-      <c r="A39" s="618" t="s">
+      <c r="A39" s="556" t="s">
         <v>255</v>
       </c>
       <c r="B39" s="47" t="s">
         <v>256</v>
       </c>
-      <c r="C39" s="76"/>
+      <c r="C39" s="626"/>
       <c r="D39" s="545"/>
       <c r="E39" s="545">
         <v>181200</v>
@@ -19786,13 +19823,13 @@
       <c r="AT39" s="332"/>
     </row>
     <row r="40" spans="1:46">
-      <c r="A40" s="618" t="s">
+      <c r="A40" s="556" t="s">
         <v>1150</v>
       </c>
       <c r="B40" s="65" t="s">
         <v>260</v>
       </c>
-      <c r="C40" s="623"/>
+      <c r="C40" s="541"/>
       <c r="D40" s="545"/>
       <c r="E40" s="545">
         <v>176200</v>
@@ -19869,14 +19906,14 @@
       <c r="AT40" s="332"/>
     </row>
     <row r="41" spans="1:46">
-      <c r="A41" s="618" t="s">
+      <c r="A41" s="556" t="s">
         <v>1151</v>
       </c>
       <c r="B41" s="65" t="s">
         <v>263</v>
       </c>
-      <c r="C41" s="623"/>
-      <c r="D41" s="622"/>
+      <c r="C41" s="630"/>
+      <c r="D41" s="560"/>
       <c r="E41" s="545">
         <v>174100</v>
       </c>
@@ -19955,14 +19992,14 @@
       <c r="AT41" s="332"/>
     </row>
     <row r="42" spans="1:46">
-      <c r="A42" s="618" t="s">
+      <c r="A42" s="556" t="s">
         <v>1152</v>
       </c>
       <c r="B42" s="65" t="s">
         <v>268</v>
       </c>
-      <c r="C42" s="623"/>
-      <c r="D42" s="622"/>
+      <c r="C42" s="630"/>
+      <c r="D42" s="560"/>
       <c r="E42" s="545">
         <v>175300</v>
       </c>
@@ -20041,14 +20078,14 @@
       <c r="AT42" s="332"/>
     </row>
     <row r="43" spans="1:46">
-      <c r="A43" s="618" t="s">
+      <c r="A43" s="556" t="s">
         <v>1153</v>
       </c>
       <c r="B43" s="65" t="s">
         <v>273</v>
       </c>
-      <c r="C43" s="623"/>
-      <c r="D43" s="622"/>
+      <c r="C43" s="630"/>
+      <c r="D43" s="560"/>
       <c r="E43" s="545">
         <v>176200</v>
       </c>
@@ -20124,14 +20161,14 @@
       <c r="AT43" s="332"/>
     </row>
     <row r="44" spans="1:46">
-      <c r="A44" s="618" t="s">
+      <c r="A44" s="556" t="s">
         <v>1154</v>
       </c>
       <c r="B44" s="65" t="s">
         <v>277</v>
       </c>
-      <c r="C44" s="623"/>
-      <c r="D44" s="622"/>
+      <c r="C44" s="630"/>
+      <c r="D44" s="560"/>
       <c r="E44" s="545">
         <v>174300</v>
       </c>
@@ -20210,14 +20247,14 @@
       <c r="AT44" s="332"/>
     </row>
     <row r="45" spans="1:46">
-      <c r="A45" s="618" t="s">
+      <c r="A45" s="556" t="s">
         <v>1155</v>
       </c>
       <c r="B45" s="65" t="s">
         <v>281</v>
       </c>
-      <c r="C45" s="623"/>
-      <c r="D45" s="622"/>
+      <c r="C45" s="626"/>
+      <c r="D45" s="560"/>
       <c r="E45" s="545">
         <v>181200</v>
       </c>
@@ -20296,13 +20333,13 @@
       <c r="AT45" s="332"/>
     </row>
     <row r="46" spans="1:46">
-      <c r="A46" s="618" t="s">
+      <c r="A46" s="556" t="s">
         <v>285</v>
       </c>
       <c r="B46" s="47" t="s">
         <v>286</v>
       </c>
-      <c r="C46" s="76"/>
+      <c r="C46" s="626"/>
       <c r="D46" s="29"/>
       <c r="E46" s="545">
         <v>173200</v>
@@ -20365,13 +20402,13 @@
       <c r="AT46" s="332"/>
     </row>
     <row r="47" spans="1:46">
-      <c r="A47" s="618" t="s">
+      <c r="A47" s="556" t="s">
         <v>1156</v>
       </c>
       <c r="B47" s="65" t="s">
         <v>291</v>
       </c>
-      <c r="C47" s="623"/>
+      <c r="C47" s="541"/>
       <c r="D47" s="29"/>
       <c r="E47" s="545">
         <v>181200</v>
@@ -20434,13 +20471,13 @@
       <c r="AT47" s="332"/>
     </row>
     <row r="48" spans="1:46">
-      <c r="A48" s="618" t="s">
+      <c r="A48" s="556" t="s">
         <v>1157</v>
       </c>
       <c r="B48" s="65" t="s">
         <v>296</v>
       </c>
-      <c r="C48" s="623"/>
+      <c r="C48" s="630"/>
       <c r="D48" s="29"/>
       <c r="E48" s="545">
         <v>739401</v>
@@ -20503,13 +20540,13 @@
       <c r="AT48" s="332"/>
     </row>
     <row r="49" spans="1:46">
-      <c r="A49" s="618" t="s">
+      <c r="A49" s="556" t="s">
         <v>1158</v>
       </c>
       <c r="B49" s="65" t="s">
         <v>300</v>
       </c>
-      <c r="C49" s="623"/>
+      <c r="C49" s="630"/>
       <c r="D49" s="29"/>
       <c r="E49" s="545">
         <v>739402</v>
@@ -20572,13 +20609,13 @@
       <c r="AT49" s="332"/>
     </row>
     <row r="50" spans="1:46">
-      <c r="A50" s="618" t="s">
+      <c r="A50" s="556" t="s">
         <v>1159</v>
       </c>
       <c r="B50" s="65" t="s">
         <v>303</v>
       </c>
-      <c r="C50" s="623"/>
+      <c r="C50" s="630"/>
       <c r="D50" s="29"/>
       <c r="E50" s="545">
         <v>152800</v>
@@ -20641,13 +20678,13 @@
       <c r="AT50" s="332"/>
     </row>
     <row r="51" spans="1:46">
-      <c r="A51" s="618" t="s">
+      <c r="A51" s="556" t="s">
         <v>1160</v>
       </c>
       <c r="B51" s="65" t="s">
         <v>307</v>
       </c>
-      <c r="C51" s="623"/>
+      <c r="C51" s="630"/>
       <c r="D51" s="29"/>
       <c r="E51" s="545">
         <v>73500</v>
@@ -20708,13 +20745,13 @@
       <c r="AT51" s="332"/>
     </row>
     <row r="52" spans="1:46">
-      <c r="A52" s="618" t="s">
+      <c r="A52" s="556" t="s">
         <v>1161</v>
       </c>
       <c r="B52" s="65" t="s">
         <v>311</v>
       </c>
-      <c r="C52" s="623"/>
+      <c r="C52" s="626"/>
       <c r="D52" s="29"/>
       <c r="E52" s="545">
         <v>152100</v>
@@ -20775,13 +20812,13 @@
       <c r="AT52" s="332"/>
     </row>
     <row r="53" spans="1:46">
-      <c r="A53" s="618" t="s">
+      <c r="A53" s="556" t="s">
         <v>315</v>
       </c>
       <c r="B53" s="47" t="s">
         <v>316</v>
       </c>
-      <c r="C53" s="76"/>
+      <c r="C53" s="626"/>
       <c r="D53" s="29"/>
       <c r="E53" s="545">
         <v>152800</v>
@@ -20842,13 +20879,13 @@
       <c r="AT53" s="332"/>
     </row>
     <row r="54" spans="1:46">
-      <c r="A54" s="618" t="s">
+      <c r="A54" s="556" t="s">
         <v>1162</v>
       </c>
       <c r="B54" s="65" t="s">
         <v>321</v>
       </c>
-      <c r="C54" s="623"/>
+      <c r="C54" s="541"/>
       <c r="D54" s="29"/>
       <c r="E54" s="545">
         <v>153500</v>
@@ -20861,7 +20898,7 @@
         <v>0</v>
       </c>
       <c r="H54" s="57">
-        <f>$C$121</f>
+        <f t="shared" ref="H54:H62" si="22">$C$121</f>
         <v>0</v>
       </c>
       <c r="I54" s="57">
@@ -20909,13 +20946,13 @@
       <c r="AT54" s="332"/>
     </row>
     <row r="55" spans="1:46">
-      <c r="A55" s="618" t="s">
+      <c r="A55" s="556" t="s">
         <v>1163</v>
       </c>
       <c r="B55" s="65" t="s">
         <v>326</v>
       </c>
-      <c r="C55" s="623"/>
+      <c r="C55" s="630"/>
       <c r="D55" s="29"/>
       <c r="E55" s="545">
         <v>175200</v>
@@ -20928,14 +20965,14 @@
         <v>0</v>
       </c>
       <c r="H55" s="57">
-        <f>$C$121</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="I55" s="57">
         <v>4</v>
       </c>
       <c r="J55" s="57">
-        <f t="shared" ref="J55:J62" si="22">IF(G55&lt;&gt;1,0,IF(H55&gt;I55,1,0))</f>
+        <f t="shared" ref="J55:J62" si="23">IF(G55&lt;&gt;1,0,IF(H55&gt;I55,1,0))</f>
         <v>0</v>
       </c>
       <c r="K55" s="57" t="s">
@@ -20976,13 +21013,13 @@
       <c r="AT55" s="332"/>
     </row>
     <row r="56" spans="1:46">
-      <c r="A56" s="618" t="s">
+      <c r="A56" s="556" t="s">
         <v>1164</v>
       </c>
       <c r="B56" s="65" t="s">
         <v>331</v>
       </c>
-      <c r="C56" s="623"/>
+      <c r="C56" s="630"/>
       <c r="D56" s="29"/>
       <c r="E56" s="545">
         <v>175300</v>
@@ -20995,14 +21032,14 @@
         <v>0</v>
       </c>
       <c r="H56" s="57">
-        <f>$C$121</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="I56" s="57">
         <v>4</v>
       </c>
       <c r="J56" s="57">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="K56" s="57" t="s">
@@ -21043,13 +21080,13 @@
       <c r="AT56" s="332"/>
     </row>
     <row r="57" spans="1:46">
-      <c r="A57" s="618" t="s">
+      <c r="A57" s="556" t="s">
         <v>1165</v>
       </c>
       <c r="B57" s="65" t="s">
         <v>335</v>
       </c>
-      <c r="C57" s="623"/>
+      <c r="C57" s="630"/>
       <c r="D57" s="29"/>
       <c r="E57" s="545">
         <v>174300</v>
@@ -21062,14 +21099,14 @@
         <v>0</v>
       </c>
       <c r="H57" s="57">
-        <f>$C$121</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="I57" s="57">
         <v>4</v>
       </c>
       <c r="J57" s="57">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="K57" s="57" t="s">
@@ -21110,13 +21147,13 @@
       <c r="AT57" s="332"/>
     </row>
     <row r="58" spans="1:46">
-      <c r="A58" s="618" t="s">
+      <c r="A58" s="556" t="s">
         <v>1166</v>
       </c>
       <c r="B58" s="65" t="s">
         <v>340</v>
       </c>
-      <c r="C58" s="623"/>
+      <c r="C58" s="630"/>
       <c r="D58" s="29"/>
       <c r="E58" s="545">
         <v>176600</v>
@@ -21129,14 +21166,14 @@
         <v>0</v>
       </c>
       <c r="H58" s="57">
-        <f>$C$121</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="I58" s="57">
         <v>4</v>
       </c>
       <c r="J58" s="57">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="K58" s="57" t="s">
@@ -21177,13 +21214,13 @@
       <c r="AT58" s="332"/>
     </row>
     <row r="59" spans="1:46">
-      <c r="A59" s="618" t="s">
+      <c r="A59" s="556" t="s">
         <v>1167</v>
       </c>
       <c r="B59" s="65" t="s">
         <v>343</v>
       </c>
-      <c r="C59" s="623"/>
+      <c r="C59" s="626"/>
       <c r="D59" s="29"/>
       <c r="E59" s="545">
         <v>175500</v>
@@ -21196,14 +21233,14 @@
         <v>0</v>
       </c>
       <c r="H59" s="57">
-        <f>$C$121</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="I59" s="57">
         <v>4</v>
       </c>
       <c r="J59" s="57">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="K59" s="57" t="s">
@@ -21244,13 +21281,13 @@
       <c r="AT59" s="332"/>
     </row>
     <row r="60" spans="1:46">
-      <c r="A60" s="618" t="s">
+      <c r="A60" s="556" t="s">
         <v>347</v>
       </c>
       <c r="B60" s="47" t="s">
         <v>348</v>
       </c>
-      <c r="C60" s="76"/>
+      <c r="C60" s="626"/>
       <c r="D60" s="29"/>
       <c r="E60" s="545">
         <v>153200</v>
@@ -21263,14 +21300,14 @@
         <v>0</v>
       </c>
       <c r="H60" s="57">
-        <f>$C$121</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="I60" s="57">
         <v>4</v>
       </c>
       <c r="J60" s="57">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="K60" s="57" t="s">
@@ -21311,13 +21348,13 @@
       <c r="AT60" s="332"/>
     </row>
     <row r="61" spans="1:46">
-      <c r="A61" s="618" t="s">
+      <c r="A61" s="556" t="s">
         <v>1168</v>
       </c>
       <c r="B61" s="65" t="s">
         <v>352</v>
       </c>
-      <c r="C61" s="623"/>
+      <c r="C61" s="541"/>
       <c r="D61" s="29"/>
       <c r="E61" s="545">
         <v>739200</v>
@@ -21330,14 +21367,14 @@
         <v>0</v>
       </c>
       <c r="H61" s="57">
-        <f>$C$121</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="I61" s="57">
         <v>4</v>
       </c>
       <c r="J61" s="57">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="K61" s="57" t="s">
@@ -21378,13 +21415,13 @@
       <c r="AT61" s="332"/>
     </row>
     <row r="62" spans="1:46">
-      <c r="A62" s="618" t="s">
+      <c r="A62" s="556" t="s">
         <v>1169</v>
       </c>
       <c r="B62" s="65" t="s">
         <v>356</v>
       </c>
-      <c r="C62" s="623"/>
+      <c r="C62" s="630"/>
       <c r="D62" s="29"/>
       <c r="E62" s="545">
         <v>174400</v>
@@ -21397,14 +21434,14 @@
         <v>0</v>
       </c>
       <c r="H62" s="57">
-        <f>$C$121</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="I62" s="57">
         <v>5</v>
       </c>
       <c r="J62" s="57">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="K62" s="57" t="s">
@@ -21445,13 +21482,13 @@
       <c r="AT62" s="332"/>
     </row>
     <row r="63" spans="1:46">
-      <c r="A63" s="618" t="s">
+      <c r="A63" s="556" t="s">
         <v>1170</v>
       </c>
       <c r="B63" s="65" t="s">
         <v>359</v>
       </c>
-      <c r="C63" s="623"/>
+      <c r="C63" s="630"/>
       <c r="D63" s="29"/>
       <c r="E63" s="545">
         <v>175400</v>
@@ -21512,13 +21549,13 @@
       <c r="AT63" s="332"/>
     </row>
     <row r="64" spans="1:46">
-      <c r="A64" s="618" t="s">
+      <c r="A64" s="556" t="s">
         <v>1171</v>
       </c>
       <c r="B64" s="65" t="s">
         <v>362</v>
       </c>
-      <c r="C64" s="623"/>
+      <c r="C64" s="630"/>
       <c r="D64" s="29"/>
       <c r="E64" s="545">
         <v>175500</v>
@@ -21579,13 +21616,13 @@
       <c r="AT64" s="332"/>
     </row>
     <row r="65" spans="1:46">
-      <c r="A65" s="618" t="s">
+      <c r="A65" s="556" t="s">
         <v>1172</v>
       </c>
       <c r="B65" s="65" t="s">
         <v>365</v>
       </c>
-      <c r="C65" s="623"/>
+      <c r="C65" s="630"/>
       <c r="D65" s="29"/>
       <c r="E65" s="545">
         <v>175500</v>
@@ -21646,13 +21683,13 @@
       <c r="AT65" s="332"/>
     </row>
     <row r="66" spans="1:46">
-      <c r="A66" s="618" t="s">
+      <c r="A66" s="556" t="s">
         <v>1173</v>
       </c>
       <c r="B66" s="65" t="s">
         <v>369</v>
       </c>
-      <c r="C66" s="623"/>
+      <c r="C66" s="626"/>
       <c r="D66" s="29"/>
       <c r="E66" s="545">
         <v>235300</v>
@@ -21713,13 +21750,13 @@
       <c r="AT66" s="332"/>
     </row>
     <row r="67" spans="1:46">
-      <c r="A67" s="618" t="s">
+      <c r="A67" s="556" t="s">
         <v>373</v>
       </c>
       <c r="B67" s="47" t="s">
         <v>374</v>
       </c>
-      <c r="C67" s="76"/>
+      <c r="C67" s="626"/>
       <c r="D67" s="29"/>
       <c r="E67" s="545">
         <v>175400</v>
@@ -21780,13 +21817,13 @@
       <c r="AT67" s="332"/>
     </row>
     <row r="68" spans="1:46">
-      <c r="A68" s="618" t="s">
+      <c r="A68" s="556" t="s">
         <v>1174</v>
       </c>
       <c r="B68" s="65" t="s">
         <v>378</v>
       </c>
-      <c r="C68" s="623"/>
+      <c r="C68" s="541"/>
       <c r="D68" s="29"/>
       <c r="E68" s="545">
         <v>175500</v>
@@ -21847,13 +21884,13 @@
       <c r="AT68" s="332"/>
     </row>
     <row r="69" spans="1:46">
-      <c r="A69" s="618" t="s">
+      <c r="A69" s="556" t="s">
         <v>1175</v>
       </c>
       <c r="B69" s="65" t="s">
         <v>382</v>
       </c>
-      <c r="C69" s="623"/>
+      <c r="C69" s="630"/>
       <c r="D69" s="29"/>
       <c r="E69" s="545">
         <v>73500</v>
@@ -21914,13 +21951,13 @@
       <c r="AT69" s="332"/>
     </row>
     <row r="70" spans="1:46">
-      <c r="A70" s="618" t="s">
+      <c r="A70" s="556" t="s">
         <v>1176</v>
       </c>
       <c r="B70" s="65" t="s">
         <v>386</v>
       </c>
-      <c r="C70" s="623"/>
+      <c r="C70" s="630"/>
       <c r="D70" s="29"/>
       <c r="E70" s="545">
         <v>73600</v>
@@ -21981,13 +22018,13 @@
       <c r="AT70" s="332"/>
     </row>
     <row r="71" spans="1:46">
-      <c r="A71" s="618" t="s">
+      <c r="A71" s="556" t="s">
         <v>1177</v>
       </c>
       <c r="B71" s="65" t="s">
         <v>389</v>
       </c>
-      <c r="C71" s="623"/>
+      <c r="C71" s="630"/>
       <c r="D71" s="29"/>
       <c r="E71" s="545"/>
       <c r="F71" s="545"/>
@@ -22055,13 +22092,13 @@
       <c r="AT71" s="332"/>
     </row>
     <row r="72" spans="1:46">
-      <c r="A72" s="618" t="s">
+      <c r="A72" s="556" t="s">
         <v>1178</v>
       </c>
       <c r="B72" s="65" t="s">
         <v>391</v>
       </c>
-      <c r="C72" s="623"/>
+      <c r="C72" s="630"/>
       <c r="D72" s="29"/>
       <c r="E72" s="545"/>
       <c r="F72" s="545"/>
@@ -22095,19 +22132,19 @@
         <v>0</v>
       </c>
       <c r="R72" s="81">
-        <f>C20</f>
+        <f>C20/100</f>
         <v>0</v>
       </c>
       <c r="S72" s="81">
-        <f>C21</f>
+        <f>C21/100</f>
         <v>0</v>
       </c>
       <c r="T72" s="81">
-        <f>C22</f>
+        <f>C22/100</f>
         <v>0</v>
       </c>
       <c r="U72" s="81">
-        <f>C23</f>
+        <f>C23/100</f>
         <v>0</v>
       </c>
       <c r="AE72" s="44" t="str">
@@ -22134,13 +22171,13 @@
       <c r="AT72" s="332"/>
     </row>
     <row r="73" spans="1:46">
-      <c r="A73" s="618" t="s">
+      <c r="A73" s="556" t="s">
         <v>1179</v>
       </c>
       <c r="B73" s="65" t="s">
         <v>394</v>
       </c>
-      <c r="C73" s="623"/>
+      <c r="C73" s="626"/>
       <c r="D73" s="29"/>
       <c r="E73" s="545"/>
       <c r="F73" s="545"/>
@@ -22174,19 +22211,19 @@
         <v>0</v>
       </c>
       <c r="R73" s="81">
-        <f>C27</f>
+        <f>C27/100</f>
         <v>0</v>
       </c>
       <c r="S73" s="81">
-        <f>C28</f>
+        <f>C28/100</f>
         <v>0</v>
       </c>
       <c r="T73" s="81">
-        <f>C29</f>
+        <f>C29/100</f>
         <v>0</v>
       </c>
       <c r="U73" s="81">
-        <f>C30</f>
+        <f>C30/100</f>
         <v>0</v>
       </c>
       <c r="AE73" s="44" t="str">
@@ -22213,13 +22250,13 @@
       <c r="AT73" s="332"/>
     </row>
     <row r="74" spans="1:46">
-      <c r="A74" s="618" t="s">
+      <c r="A74" s="556" t="s">
         <v>397</v>
       </c>
       <c r="B74" s="47" t="s">
         <v>398</v>
       </c>
-      <c r="C74" s="76"/>
+      <c r="C74" s="626"/>
       <c r="D74" s="29"/>
       <c r="E74" s="545"/>
       <c r="F74" s="545"/>
@@ -22253,19 +22290,19 @@
         <v>0</v>
       </c>
       <c r="R74" s="81">
-        <f>C34</f>
+        <f>C34/100</f>
         <v>0</v>
       </c>
       <c r="S74" s="81">
-        <f>C35</f>
+        <f>C35/100</f>
         <v>0</v>
       </c>
       <c r="T74" s="81">
-        <f>C36</f>
+        <f>C36/100</f>
         <v>0</v>
       </c>
       <c r="U74" s="81">
-        <f>C37</f>
+        <f>C37/100</f>
         <v>0</v>
       </c>
       <c r="AE74" s="44" t="str">
@@ -22292,13 +22329,13 @@
       <c r="AT74" s="332"/>
     </row>
     <row r="75" spans="1:46">
-      <c r="A75" s="618" t="s">
+      <c r="A75" s="556" t="s">
         <v>1180</v>
       </c>
       <c r="B75" s="79" t="s">
         <v>400</v>
       </c>
-      <c r="C75" s="624"/>
+      <c r="C75" s="541"/>
       <c r="D75" s="29"/>
       <c r="E75" s="545"/>
       <c r="F75" s="545"/>
@@ -22332,19 +22369,19 @@
         <v>0</v>
       </c>
       <c r="R75" s="81">
-        <f>C41</f>
+        <f>C41/100</f>
         <v>0</v>
       </c>
       <c r="S75" s="81">
-        <f>C42</f>
+        <f>C42/100</f>
         <v>0</v>
       </c>
       <c r="T75" s="81">
-        <f>C43</f>
+        <f>C43/100</f>
         <v>0</v>
       </c>
       <c r="U75" s="81">
-        <f>C44</f>
+        <f>C44/100</f>
         <v>0</v>
       </c>
       <c r="AE75" s="44" t="s">
@@ -22370,13 +22407,13 @@
       <c r="AT75" s="332"/>
     </row>
     <row r="76" spans="1:46">
-      <c r="A76" s="618" t="s">
+      <c r="A76" s="556" t="s">
         <v>1181</v>
       </c>
       <c r="B76" s="65" t="s">
         <v>402</v>
       </c>
-      <c r="C76" s="623"/>
+      <c r="C76" s="630"/>
       <c r="D76" s="29"/>
       <c r="E76" s="545"/>
       <c r="F76" s="545"/>
@@ -22410,19 +22447,19 @@
         <v>0</v>
       </c>
       <c r="R76" s="40">
-        <f>C48</f>
+        <f>C48/100</f>
         <v>0</v>
       </c>
       <c r="S76" s="81">
-        <f>C49</f>
+        <f>C49/100</f>
         <v>0</v>
       </c>
       <c r="T76" s="81">
-        <f>C50</f>
+        <f>C50/100</f>
         <v>0</v>
       </c>
       <c r="U76" s="81">
-        <f>C51</f>
+        <f>C51/100</f>
         <v>0</v>
       </c>
       <c r="AE76" s="44" t="str">
@@ -22449,13 +22486,13 @@
       <c r="AT76" s="332"/>
     </row>
     <row r="77" spans="1:46">
-      <c r="A77" s="618" t="s">
+      <c r="A77" s="556" t="s">
         <v>1182</v>
       </c>
       <c r="B77" s="65" t="s">
         <v>411</v>
       </c>
-      <c r="C77" s="623"/>
+      <c r="C77" s="630"/>
       <c r="D77" s="29"/>
       <c r="E77" s="545"/>
       <c r="F77" s="545"/>
@@ -22489,19 +22526,19 @@
         <v>0</v>
       </c>
       <c r="R77" s="81">
-        <f>C55</f>
+        <f>C55/100</f>
         <v>0</v>
       </c>
       <c r="S77" s="81">
-        <f>C56</f>
+        <f>C56/100</f>
         <v>0</v>
       </c>
       <c r="T77" s="81">
-        <f>C57</f>
+        <f>C57/100</f>
         <v>0</v>
       </c>
       <c r="U77" s="81">
-        <f>C58</f>
+        <f>C58/100</f>
         <v>0</v>
       </c>
       <c r="AE77" s="44"/>
@@ -22520,13 +22557,13 @@
       <c r="AT77" s="332"/>
     </row>
     <row r="78" spans="1:46">
-      <c r="A78" s="618" t="s">
+      <c r="A78" s="556" t="s">
         <v>1183</v>
       </c>
       <c r="B78" s="65" t="s">
         <v>414</v>
       </c>
-      <c r="C78" s="623"/>
+      <c r="C78" s="630"/>
       <c r="D78" s="29"/>
       <c r="E78" s="545"/>
       <c r="F78" s="545"/>
@@ -22560,19 +22597,19 @@
         <v>0</v>
       </c>
       <c r="R78" s="81">
-        <f>C62</f>
+        <f>C62/100</f>
         <v>0</v>
       </c>
       <c r="S78" s="81">
-        <f>C63</f>
+        <f>C63/100</f>
         <v>0</v>
       </c>
       <c r="T78" s="81">
-        <f>C64</f>
+        <f>C64/100</f>
         <v>0</v>
       </c>
       <c r="U78" s="81">
-        <f>C65</f>
+        <f>C65/100</f>
         <v>0</v>
       </c>
       <c r="AE78" s="44" t="str">
@@ -22593,19 +22630,19 @@
         <v>361</v>
       </c>
       <c r="AJ78" s="40" t="str">
-        <f t="shared" ref="AJ78:AJ141" si="23">IFERROR(IF($AJ$7&lt;&gt;"Quote","",IF(VLOOKUP(AI78,$AF$7:$AG$240,2,FALSE)=0,"-",VLOOKUP(AI78,$AF$7:$AG$240,2,FALSE))),"-")</f>
+        <f t="shared" ref="AJ78:AJ141" si="24">IFERROR(IF($AJ$7&lt;&gt;"Quote","",IF(VLOOKUP(AI78,$AF$7:$AG$240,2,FALSE)=0,"-",VLOOKUP(AI78,$AF$7:$AG$240,2,FALSE))),"-")</f>
         <v/>
       </c>
       <c r="AT78" s="332"/>
     </row>
     <row r="79" spans="1:46">
-      <c r="A79" s="618" t="s">
+      <c r="A79" s="556" t="s">
         <v>1184</v>
       </c>
       <c r="B79" s="65" t="s">
         <v>417</v>
       </c>
-      <c r="C79" s="623"/>
+      <c r="C79" s="630"/>
       <c r="D79" s="29"/>
       <c r="E79" s="545"/>
       <c r="F79" s="545"/>
@@ -22639,19 +22676,19 @@
         <v>0</v>
       </c>
       <c r="R79" s="81">
-        <f>C69</f>
+        <f>C69/100</f>
         <v>0</v>
       </c>
       <c r="S79" s="81">
-        <f>C70</f>
+        <f>C70/100</f>
         <v>0</v>
       </c>
       <c r="T79" s="81">
-        <f>C71</f>
+        <f>C71/100</f>
         <v>0</v>
       </c>
       <c r="U79" s="81">
-        <f>C72</f>
+        <f>C72/100</f>
         <v>0</v>
       </c>
       <c r="AE79" s="44" t="str">
@@ -22672,19 +22709,19 @@
         <v>364</v>
       </c>
       <c r="AJ79" s="40" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="AT79" s="332"/>
     </row>
     <row r="80" spans="1:46">
-      <c r="A80" s="618" t="s">
+      <c r="A80" s="556" t="s">
         <v>1185</v>
       </c>
       <c r="B80" s="65" t="s">
         <v>420</v>
       </c>
-      <c r="C80" s="623"/>
+      <c r="C80" s="626"/>
       <c r="D80" s="29"/>
       <c r="E80" s="545"/>
       <c r="F80" s="545"/>
@@ -22718,19 +22755,19 @@
         <v>0</v>
       </c>
       <c r="R80" s="81">
-        <f>C76</f>
+        <f>C76/100</f>
         <v>0</v>
       </c>
       <c r="S80" s="81">
-        <f>C77</f>
+        <f>C77/100</f>
         <v>0</v>
       </c>
       <c r="T80" s="81">
-        <f>C78</f>
+        <f>C78/100</f>
         <v>0</v>
       </c>
       <c r="U80" s="81">
-        <f>C79</f>
+        <f>C79/100</f>
         <v>0</v>
       </c>
       <c r="AE80" s="44" t="str">
@@ -22751,19 +22788,19 @@
         <v>457</v>
       </c>
       <c r="AJ80" s="40" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="AT80" s="332"/>
     </row>
     <row r="81" spans="1:46" ht="15" thickBot="1">
-      <c r="A81" s="618" t="s">
+      <c r="A81" s="556" t="s">
         <v>424</v>
       </c>
       <c r="B81" s="47" t="s">
         <v>425</v>
       </c>
-      <c r="C81" s="76"/>
+      <c r="C81" s="626"/>
       <c r="D81" s="29"/>
       <c r="E81" s="545"/>
       <c r="F81" s="545"/>
@@ -22797,19 +22834,19 @@
         <v>0</v>
       </c>
       <c r="R81" s="81">
-        <f>C83</f>
+        <f>C83/100</f>
         <v>0</v>
       </c>
       <c r="S81" s="81">
-        <f>C84</f>
+        <f>C84/100</f>
         <v>0</v>
       </c>
       <c r="T81" s="81">
-        <f>C85</f>
+        <f>C85/100</f>
         <v>0</v>
       </c>
       <c r="U81" s="81">
-        <f>C86</f>
+        <f>C86/100</f>
         <v>0</v>
       </c>
       <c r="AE81" s="44" t="str">
@@ -22830,19 +22867,19 @@
         <v>461</v>
       </c>
       <c r="AJ81" s="40" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="AT81" s="332"/>
     </row>
     <row r="82" spans="1:46" ht="15" thickTop="1">
-      <c r="A82" s="618" t="s">
+      <c r="A82" s="556" t="s">
         <v>1186</v>
       </c>
       <c r="B82" s="65" t="s">
         <v>428</v>
       </c>
-      <c r="C82" s="623"/>
+      <c r="C82" s="541"/>
       <c r="D82" s="29"/>
       <c r="E82" s="545"/>
       <c r="F82" s="545"/>
@@ -22910,19 +22947,19 @@
         <v>367</v>
       </c>
       <c r="AJ82" s="40" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="AT82" s="332"/>
     </row>
     <row r="83" spans="1:46">
-      <c r="A83" s="618" t="s">
+      <c r="A83" s="556" t="s">
         <v>1187</v>
       </c>
       <c r="B83" s="65" t="s">
         <v>431</v>
       </c>
-      <c r="C83" s="623"/>
+      <c r="C83" s="630"/>
       <c r="D83" s="29"/>
       <c r="E83" s="545"/>
       <c r="F83" s="545"/>
@@ -22965,19 +23002,19 @@
         <v>465</v>
       </c>
       <c r="AJ83" s="40" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="AT83" s="332"/>
     </row>
     <row r="84" spans="1:46">
-      <c r="A84" s="618" t="s">
+      <c r="A84" s="556" t="s">
         <v>1188</v>
       </c>
       <c r="B84" s="65" t="s">
         <v>435</v>
       </c>
-      <c r="C84" s="623"/>
+      <c r="C84" s="630"/>
       <c r="D84" s="29"/>
       <c r="E84" s="545"/>
       <c r="F84" s="545"/>
@@ -23016,19 +23053,19 @@
         <v>371</v>
       </c>
       <c r="AJ84" s="40" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="AT84" s="332"/>
     </row>
     <row r="85" spans="1:46">
-      <c r="A85" s="618" t="s">
+      <c r="A85" s="556" t="s">
         <v>1189</v>
       </c>
       <c r="B85" s="65" t="s">
         <v>439</v>
       </c>
-      <c r="C85" s="623"/>
+      <c r="C85" s="630"/>
       <c r="D85" s="29"/>
       <c r="E85" s="545"/>
       <c r="F85" s="545"/>
@@ -23088,18 +23125,18 @@
         <v>376</v>
       </c>
       <c r="AJ85" s="40" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
     </row>
     <row r="86" spans="1:46">
-      <c r="A86" s="618" t="s">
+      <c r="A86" s="556" t="s">
         <v>1190</v>
       </c>
       <c r="B86" s="65" t="s">
         <v>442</v>
       </c>
-      <c r="C86" s="623"/>
+      <c r="C86" s="630"/>
       <c r="D86" s="29"/>
       <c r="O86" s="22" t="s">
         <v>459</v>
@@ -23122,7 +23159,7 @@
         <v>0</v>
       </c>
       <c r="AE86" s="554" t="str">
-        <f t="shared" ref="AE86:AE88" si="24">B92</f>
+        <f t="shared" ref="AE86:AE88" si="25">B92</f>
         <v>EDP systems limit</v>
       </c>
       <c r="AF86" s="555"/>
@@ -23137,18 +23174,18 @@
         <v>472</v>
       </c>
       <c r="AJ86" s="40" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
     </row>
     <row r="87" spans="1:46">
-      <c r="A87" s="618" t="s">
+      <c r="A87" s="556" t="s">
         <v>1191</v>
       </c>
       <c r="B87" s="65" t="s">
         <v>446</v>
       </c>
-      <c r="C87" s="623"/>
+      <c r="C87" s="626"/>
       <c r="D87" s="29"/>
       <c r="O87" s="22" t="s">
         <v>463</v>
@@ -23171,7 +23208,7 @@
         <v>0</v>
       </c>
       <c r="AE87" s="554" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>Stock limit</v>
       </c>
       <c r="AF87" s="555"/>
@@ -23186,18 +23223,18 @@
         <v>474</v>
       </c>
       <c r="AJ87" s="40" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
     </row>
     <row r="88" spans="1:46">
-      <c r="A88" s="618" t="s">
+      <c r="A88" s="556" t="s">
         <v>1192</v>
       </c>
       <c r="B88" s="65" t="s">
         <v>448</v>
       </c>
-      <c r="C88" s="623"/>
+      <c r="C88" s="631"/>
       <c r="D88" s="29"/>
       <c r="R88" s="28">
         <v>10000</v>
@@ -23210,7 +23247,7 @@
       </c>
       <c r="U88" s="64"/>
       <c r="AE88" s="554" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>Business equipment limit</v>
       </c>
       <c r="AF88" s="555"/>
@@ -23225,18 +23262,18 @@
         <v>381</v>
       </c>
       <c r="AJ88" s="40" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
     </row>
     <row r="89" spans="1:46">
-      <c r="A89" s="619">
+      <c r="A89" s="557">
         <v>1000130</v>
       </c>
       <c r="B89" s="86" t="s">
         <v>449</v>
       </c>
-      <c r="C89" s="623"/>
+      <c r="C89" s="631"/>
       <c r="D89" s="29"/>
       <c r="R89" s="28">
         <v>15000</v>
@@ -23261,18 +23298,18 @@
         <v>478</v>
       </c>
       <c r="AJ89" s="40" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
     </row>
     <row r="90" spans="1:46">
-      <c r="A90" s="619">
+      <c r="A90" s="557">
         <v>1000140</v>
       </c>
       <c r="B90" s="86" t="s">
         <v>451</v>
       </c>
-      <c r="C90" s="623"/>
+      <c r="C90" s="631"/>
       <c r="D90" s="29"/>
       <c r="R90" s="28">
         <v>25000</v>
@@ -23296,18 +23333,18 @@
         <v>86</v>
       </c>
       <c r="AJ90" s="40" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
     </row>
     <row r="91" spans="1:46">
-      <c r="A91" s="618" t="s">
+      <c r="A91" s="556" t="s">
         <v>1193</v>
       </c>
       <c r="B91" s="86" t="s">
         <v>458</v>
       </c>
-      <c r="C91" s="623"/>
+      <c r="C91" s="632"/>
       <c r="D91" s="29"/>
       <c r="R91" s="28">
         <v>35000</v>
@@ -23331,18 +23368,18 @@
         <v>384</v>
       </c>
       <c r="AJ91" s="40" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
     </row>
     <row r="92" spans="1:46">
-      <c r="A92" s="618" t="s">
+      <c r="A92" s="556" t="s">
         <v>1194</v>
       </c>
       <c r="B92" s="86" t="s">
         <v>462</v>
       </c>
-      <c r="C92" s="623"/>
+      <c r="C92" s="632"/>
       <c r="D92" s="29"/>
       <c r="R92" s="28">
         <v>50000</v>
@@ -23366,18 +23403,18 @@
         <v>388</v>
       </c>
       <c r="AJ92" s="40" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
     </row>
     <row r="93" spans="1:46">
-      <c r="A93" s="618" t="s">
+      <c r="A93" s="556" t="s">
         <v>1195</v>
       </c>
       <c r="B93" s="86" t="s">
         <v>464</v>
       </c>
-      <c r="C93" s="623"/>
+      <c r="C93" s="632"/>
       <c r="D93" s="29"/>
       <c r="R93" s="28" t="s">
         <v>471</v>
@@ -23401,18 +23438,18 @@
         <v>390</v>
       </c>
       <c r="AJ93" s="40" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
     </row>
     <row r="94" spans="1:46">
-      <c r="A94" s="618" t="s">
+      <c r="A94" s="556" t="s">
         <v>1196</v>
       </c>
       <c r="B94" s="86" t="s">
         <v>466</v>
       </c>
-      <c r="C94" s="623"/>
+      <c r="C94" s="632"/>
       <c r="D94" s="29"/>
       <c r="R94" s="28"/>
       <c r="T94" s="28"/>
@@ -23429,18 +23466,18 @@
         <v>484</v>
       </c>
       <c r="AJ94" s="40" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
     </row>
     <row r="95" spans="1:46">
-      <c r="A95" s="619">
+      <c r="A95" s="557">
         <v>1000160</v>
       </c>
       <c r="B95" s="86" t="s">
         <v>467</v>
       </c>
-      <c r="C95" s="623"/>
+      <c r="C95" s="631"/>
       <c r="D95" s="29"/>
       <c r="R95" s="28"/>
       <c r="T95" s="28"/>
@@ -23457,18 +23494,18 @@
         <v>487</v>
       </c>
       <c r="AJ95" s="40" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
     </row>
     <row r="96" spans="1:46">
-      <c r="A96" s="618" t="s">
+      <c r="A96" s="556" t="s">
         <v>1197</v>
       </c>
       <c r="B96" s="86" t="s">
         <v>468</v>
       </c>
-      <c r="C96" s="623"/>
+      <c r="C96" s="625"/>
       <c r="D96" s="29"/>
       <c r="O96" s="80" t="s">
         <v>477</v>
@@ -23488,18 +23525,18 @@
         <v>489</v>
       </c>
       <c r="AJ96" s="40" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
     </row>
     <row r="97" spans="1:36">
-      <c r="A97" s="619">
+      <c r="A97" s="557">
         <v>1000100</v>
       </c>
       <c r="B97" s="86" t="s">
         <v>469</v>
       </c>
-      <c r="C97" s="623"/>
+      <c r="C97" s="633"/>
       <c r="D97" s="29"/>
       <c r="O97" s="87" t="s">
         <v>452</v>
@@ -23532,18 +23569,18 @@
         <v>395</v>
       </c>
       <c r="AJ97" s="40" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
     </row>
     <row r="98" spans="1:36">
-      <c r="A98" s="619" t="s">
+      <c r="A98" s="557" t="s">
         <v>1198</v>
       </c>
       <c r="B98" s="86" t="s">
         <v>470</v>
       </c>
-      <c r="C98" s="623"/>
+      <c r="C98" s="631"/>
       <c r="D98" s="29"/>
       <c r="O98" s="22" t="s">
         <v>480</v>
@@ -23583,18 +23620,18 @@
         <v>209</v>
       </c>
       <c r="AJ98" s="40" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
     </row>
     <row r="99" spans="1:36">
-      <c r="A99" s="619">
+      <c r="A99" s="557">
         <v>1000360</v>
       </c>
       <c r="B99" s="86" t="s">
         <v>473</v>
       </c>
-      <c r="C99" s="623"/>
+      <c r="C99" s="541"/>
       <c r="D99" s="29"/>
       <c r="O99" s="22" t="s">
         <v>463</v>
@@ -23634,18 +23671,18 @@
         <v>156</v>
       </c>
       <c r="AJ99" s="40" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
     </row>
     <row r="100" spans="1:36">
-      <c r="A100" s="619">
+      <c r="A100" s="557">
         <v>1000190</v>
       </c>
       <c r="B100" s="86" t="s">
         <v>475</v>
       </c>
-      <c r="C100" s="623"/>
+      <c r="C100" s="631"/>
       <c r="D100" s="29"/>
       <c r="Q100" s="95"/>
       <c r="R100" s="28">
@@ -23671,18 +23708,18 @@
         <v>492</v>
       </c>
       <c r="AJ100" s="40" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
     </row>
     <row r="101" spans="1:36">
-      <c r="A101" s="619" t="s">
+      <c r="A101" s="557" t="s">
         <v>1199</v>
       </c>
       <c r="B101" s="86" t="s">
         <v>476</v>
       </c>
-      <c r="C101" s="623"/>
+      <c r="C101" s="631"/>
       <c r="D101" s="29"/>
       <c r="Q101" s="95"/>
       <c r="R101" s="28">
@@ -23708,18 +23745,18 @@
         <v>493</v>
       </c>
       <c r="AJ101" s="40" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
     </row>
     <row r="102" spans="1:36">
-      <c r="A102" s="619">
+      <c r="A102" s="557">
         <v>1000220</v>
       </c>
       <c r="B102" s="86" t="s">
         <v>479</v>
       </c>
-      <c r="C102" s="623"/>
+      <c r="C102" s="631"/>
       <c r="D102" s="29"/>
       <c r="Q102" s="95"/>
       <c r="R102" s="28">
@@ -23745,18 +23782,18 @@
         <v>494</v>
       </c>
       <c r="AJ102" s="40" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
     </row>
     <row r="103" spans="1:36">
-      <c r="A103" s="619">
+      <c r="A103" s="557">
         <v>1000210</v>
       </c>
       <c r="B103" s="86" t="s">
         <v>481</v>
       </c>
-      <c r="C103" s="623"/>
+      <c r="C103" s="631"/>
       <c r="D103" s="29"/>
       <c r="Q103" s="95"/>
       <c r="R103" s="28">
@@ -23782,18 +23819,18 @@
         <v>183</v>
       </c>
       <c r="AJ103" s="40" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
     </row>
     <row r="104" spans="1:36">
-      <c r="A104" s="619" t="s">
+      <c r="A104" s="557" t="s">
         <v>1200</v>
       </c>
       <c r="B104" s="86" t="s">
         <v>482</v>
       </c>
-      <c r="C104" s="623"/>
+      <c r="C104" s="631"/>
       <c r="D104" s="29"/>
       <c r="R104" s="28">
         <v>25000</v>
@@ -23817,18 +23854,18 @@
         <v>1113</v>
       </c>
       <c r="AJ104" s="40" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
     </row>
     <row r="105" spans="1:36">
-      <c r="A105" s="619">
+      <c r="A105" s="557">
         <v>1000380</v>
       </c>
       <c r="B105" s="86" t="s">
         <v>483</v>
       </c>
-      <c r="C105" s="623"/>
+      <c r="C105" s="541"/>
       <c r="D105" s="29"/>
       <c r="R105" s="28">
         <v>35000</v>
@@ -23852,18 +23889,18 @@
         <v>496</v>
       </c>
       <c r="AJ105" s="40" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
     </row>
     <row r="106" spans="1:36">
-      <c r="A106" s="619">
+      <c r="A106" s="557">
         <v>1000180</v>
       </c>
       <c r="B106" s="86" t="s">
         <v>485</v>
       </c>
-      <c r="C106" s="623"/>
+      <c r="C106" s="631"/>
       <c r="D106" s="29"/>
       <c r="R106" s="28">
         <v>50000</v>
@@ -23887,18 +23924,18 @@
         <v>498</v>
       </c>
       <c r="AJ106" s="40" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
     </row>
     <row r="107" spans="1:36">
-      <c r="A107" s="619" t="s">
+      <c r="A107" s="557" t="s">
         <v>1201</v>
       </c>
       <c r="B107" s="86" t="s">
         <v>486</v>
       </c>
-      <c r="C107" s="623"/>
+      <c r="C107" s="631"/>
       <c r="D107" s="29"/>
       <c r="R107" s="28">
         <v>100000</v>
@@ -23922,18 +23959,18 @@
         <v>399</v>
       </c>
       <c r="AJ107" s="40" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
     </row>
     <row r="108" spans="1:36">
-      <c r="A108" s="619">
+      <c r="A108" s="557">
         <v>1000310</v>
       </c>
       <c r="B108" s="86" t="s">
         <v>488</v>
       </c>
-      <c r="C108" s="623"/>
+      <c r="C108" s="631"/>
       <c r="D108" s="29"/>
       <c r="R108" s="28" t="s">
         <v>471</v>
@@ -23957,18 +23994,18 @@
         <v>401</v>
       </c>
       <c r="AJ108" s="40" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
     </row>
     <row r="109" spans="1:36">
-      <c r="A109" s="619" t="s">
+      <c r="A109" s="557" t="s">
         <v>1202</v>
       </c>
       <c r="B109" s="86" t="s">
         <v>490</v>
       </c>
-      <c r="C109" s="623"/>
+      <c r="C109" s="631"/>
       <c r="D109" s="29"/>
       <c r="R109" s="28"/>
       <c r="T109" s="28"/>
@@ -23985,18 +24022,18 @@
         <v>409</v>
       </c>
       <c r="AJ109" s="40" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
     </row>
     <row r="110" spans="1:36">
-      <c r="A110" s="619">
+      <c r="A110" s="557">
         <v>1000300</v>
       </c>
       <c r="B110" s="86" t="s">
         <v>491</v>
       </c>
-      <c r="C110" s="623"/>
+      <c r="C110" s="541"/>
       <c r="D110" s="29"/>
       <c r="R110" s="28"/>
       <c r="T110" s="28"/>
@@ -24013,18 +24050,18 @@
         <v>173</v>
       </c>
       <c r="AJ110" s="40" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
     </row>
     <row r="111" spans="1:36">
-      <c r="A111" s="619">
+      <c r="A111" s="557">
         <v>10001</v>
       </c>
       <c r="B111" s="86" t="s">
         <v>1093</v>
       </c>
-      <c r="C111" s="76"/>
+      <c r="C111" s="541"/>
       <c r="D111" s="29"/>
       <c r="O111" s="80" t="s">
         <v>495</v>
@@ -24041,18 +24078,18 @@
         <v>499</v>
       </c>
       <c r="AJ111" s="40" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
     </row>
     <row r="112" spans="1:36">
-      <c r="A112" s="619">
+      <c r="A112" s="557">
         <v>11001</v>
       </c>
       <c r="B112" s="45" t="s">
         <v>1094</v>
       </c>
-      <c r="C112" s="47"/>
+      <c r="C112" s="541"/>
       <c r="O112" s="87" t="s">
         <v>452</v>
       </c>
@@ -24081,18 +24118,18 @@
         <v>192</v>
       </c>
       <c r="AJ112" s="40" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
     </row>
     <row r="113" spans="1:36">
-      <c r="A113" s="619">
+      <c r="A113" s="557">
         <v>11045</v>
       </c>
       <c r="B113" s="45" t="s">
         <v>1109</v>
       </c>
-      <c r="C113" s="47"/>
+      <c r="C113" s="541"/>
       <c r="O113" s="22" t="s">
         <v>120</v>
       </c>
@@ -24120,18 +24157,18 @@
         <v>413</v>
       </c>
       <c r="AJ113" s="40" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
     </row>
     <row r="114" spans="1:36">
-      <c r="A114" s="619">
+      <c r="A114" s="557">
         <v>14500</v>
       </c>
       <c r="B114" s="45" t="s">
         <v>1096</v>
       </c>
-      <c r="C114" s="47"/>
+      <c r="C114" s="541"/>
       <c r="O114" s="22" t="s">
         <v>463</v>
       </c>
@@ -24162,18 +24199,18 @@
         <v>1114</v>
       </c>
       <c r="AJ114" s="40" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
     </row>
     <row r="115" spans="1:36">
-      <c r="A115" s="619">
+      <c r="A115" s="557">
         <v>13720</v>
       </c>
       <c r="B115" s="45" t="s">
         <v>1097</v>
       </c>
-      <c r="C115" s="47"/>
+      <c r="C115" s="541"/>
       <c r="R115" s="28">
         <v>5000</v>
       </c>
@@ -24193,18 +24230,18 @@
         <v>501</v>
       </c>
       <c r="AJ115" s="40" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
     </row>
     <row r="116" spans="1:36">
-      <c r="A116" s="619">
+      <c r="A116" s="557">
         <v>12720</v>
       </c>
       <c r="B116" s="45" t="s">
         <v>1098</v>
       </c>
-      <c r="C116" s="47"/>
+      <c r="C116" s="541"/>
       <c r="R116" s="28">
         <v>10000</v>
       </c>
@@ -24224,18 +24261,18 @@
         <v>503</v>
       </c>
       <c r="AJ116" s="40" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
     </row>
     <row r="117" spans="1:36">
-      <c r="A117" s="619">
+      <c r="A117" s="557">
         <v>11920</v>
       </c>
       <c r="B117" s="45" t="s">
         <v>1099</v>
       </c>
-      <c r="C117" s="47"/>
+      <c r="C117" s="541"/>
       <c r="R117" s="28">
         <v>25000</v>
       </c>
@@ -24255,18 +24292,18 @@
         <v>201</v>
       </c>
       <c r="AJ117" s="40" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
     </row>
     <row r="118" spans="1:36">
-      <c r="A118" s="619">
+      <c r="A118" s="557">
         <v>12800</v>
       </c>
       <c r="B118" s="45" t="s">
         <v>1100</v>
       </c>
-      <c r="C118" s="47"/>
+      <c r="C118" s="541"/>
       <c r="R118" s="28">
         <v>50000</v>
       </c>
@@ -24286,18 +24323,18 @@
         <v>416</v>
       </c>
       <c r="AJ118" s="40" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
     </row>
     <row r="119" spans="1:36">
-      <c r="A119" s="619">
+      <c r="A119" s="557">
         <v>13320</v>
       </c>
       <c r="B119" s="45" t="s">
         <v>1101</v>
       </c>
-      <c r="C119" s="47"/>
+      <c r="C119" s="541"/>
       <c r="R119" s="28" t="s">
         <v>471</v>
       </c>
@@ -24317,18 +24354,18 @@
         <v>419</v>
       </c>
       <c r="AJ119" s="40" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
     </row>
     <row r="120" spans="1:36">
-      <c r="A120" s="619">
+      <c r="A120" s="557">
         <v>14550</v>
       </c>
       <c r="B120" s="45" t="s">
         <v>1102</v>
       </c>
-      <c r="C120" s="47"/>
+      <c r="C120" s="541"/>
       <c r="R120" s="28"/>
       <c r="T120" s="28"/>
       <c r="AE120" s="44"/>
@@ -24341,18 +24378,18 @@
         <v>422</v>
       </c>
       <c r="AJ120" s="40" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
     </row>
     <row r="121" spans="1:36">
-      <c r="A121" s="619">
+      <c r="A121" s="557">
         <v>13000</v>
       </c>
       <c r="B121" s="45" t="s">
         <v>1095</v>
       </c>
-      <c r="C121" s="47"/>
+      <c r="C121" s="541"/>
       <c r="O121" s="80" t="s">
         <v>500</v>
       </c>
@@ -24368,18 +24405,18 @@
         <v>427</v>
       </c>
       <c r="AJ121" s="40" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
     </row>
     <row r="122" spans="1:36">
-      <c r="A122" s="619">
+      <c r="A122" s="557">
         <v>11710</v>
       </c>
       <c r="B122" s="45" t="s">
         <v>1103</v>
       </c>
-      <c r="C122" s="47"/>
+      <c r="C122" s="541"/>
       <c r="O122" s="87" t="s">
         <v>452</v>
       </c>
@@ -24408,18 +24445,18 @@
         <v>430</v>
       </c>
       <c r="AJ122" s="40" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
     </row>
     <row r="123" spans="1:36">
-      <c r="A123" s="619">
+      <c r="A123" s="557">
         <v>11705</v>
       </c>
       <c r="B123" s="45" t="s">
         <v>1106</v>
       </c>
-      <c r="C123" s="47"/>
+      <c r="C123" s="541"/>
       <c r="O123" s="22" t="s">
         <v>129</v>
       </c>
@@ -24450,12 +24487,12 @@
         <v>433</v>
       </c>
       <c r="AJ123" s="40" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
     </row>
     <row r="124" spans="1:36">
-      <c r="A124" s="619">
+      <c r="A124" s="557">
         <v>11715</v>
       </c>
       <c r="B124" s="45" t="s">
@@ -24492,12 +24529,12 @@
         <v>1040</v>
       </c>
       <c r="AJ124" s="40" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
     </row>
     <row r="125" spans="1:36">
-      <c r="A125" s="619">
+      <c r="A125" s="557">
         <v>14580</v>
       </c>
       <c r="B125" s="45" t="s">
@@ -24531,12 +24568,12 @@
         <v>437</v>
       </c>
       <c r="AJ125" s="40" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
     </row>
     <row r="126" spans="1:36">
-      <c r="A126" s="619">
+      <c r="A126" s="557">
         <v>13900</v>
       </c>
       <c r="B126" s="45" t="s">
@@ -24570,12 +24607,12 @@
         <v>164</v>
       </c>
       <c r="AJ126" s="40" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
     </row>
     <row r="127" spans="1:36">
-      <c r="A127" s="619">
+      <c r="A127" s="557">
         <v>13910</v>
       </c>
       <c r="B127" s="45" t="s">
@@ -24608,7 +24645,7 @@
         <v>507</v>
       </c>
       <c r="AJ127" s="40" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
     </row>
@@ -24640,7 +24677,7 @@
         <v>508</v>
       </c>
       <c r="AJ128" s="40" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
     </row>
@@ -24665,7 +24702,7 @@
         <v>1115</v>
       </c>
       <c r="AJ129" s="40" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
     </row>
@@ -24690,7 +24727,7 @@
         <v>509</v>
       </c>
       <c r="AJ130" s="40" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
     </row>
@@ -24714,7 +24751,7 @@
         <v>510</v>
       </c>
       <c r="AJ131" s="40" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
     </row>
@@ -24731,7 +24768,7 @@
         <v>441</v>
       </c>
       <c r="AJ132" s="40" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
     </row>
@@ -24751,7 +24788,7 @@
         <v>511</v>
       </c>
       <c r="AJ133" s="40" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
     </row>
@@ -24784,7 +24821,7 @@
         <v>512</v>
       </c>
       <c r="AJ134" s="40" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
     </row>
@@ -24819,7 +24856,7 @@
         <v>513</v>
       </c>
       <c r="AJ135" s="40" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
     </row>
@@ -24854,7 +24891,7 @@
         <v>514</v>
       </c>
       <c r="AJ136" s="40" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
     </row>
@@ -24878,7 +24915,7 @@
         <v>516</v>
       </c>
       <c r="AJ137" s="40" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
     </row>
@@ -24902,7 +24939,7 @@
         <v>517</v>
       </c>
       <c r="AJ138" s="40" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
     </row>
@@ -24926,7 +24963,7 @@
         <v>519</v>
       </c>
       <c r="AJ139" s="40" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
     </row>
@@ -24950,7 +24987,7 @@
         <v>521</v>
       </c>
       <c r="AJ140" s="40" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
     </row>
@@ -24974,7 +25011,7 @@
         <v>523</v>
       </c>
       <c r="AJ141" s="40" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
     </row>
@@ -24991,7 +25028,7 @@
         <v>525</v>
       </c>
       <c r="AJ142" s="40" t="str">
-        <f t="shared" ref="AJ142:AJ201" si="25">IFERROR(IF($AJ$7&lt;&gt;"Quote","",IF(VLOOKUP(AI142,$AF$7:$AG$240,2,FALSE)=0,"-",VLOOKUP(AI142,$AF$7:$AG$240,2,FALSE))),"-")</f>
+        <f t="shared" ref="AJ142:AJ201" si="26">IFERROR(IF($AJ$7&lt;&gt;"Quote","",IF(VLOOKUP(AI142,$AF$7:$AG$240,2,FALSE)=0,"-",VLOOKUP(AI142,$AF$7:$AG$240,2,FALSE))),"-")</f>
         <v/>
       </c>
     </row>
@@ -25008,7 +25045,7 @@
         <v>526</v>
       </c>
       <c r="AJ143" s="40" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v/>
       </c>
     </row>
@@ -25028,7 +25065,7 @@
         <v>527</v>
       </c>
       <c r="AJ144" s="40" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v/>
       </c>
     </row>
@@ -25061,7 +25098,7 @@
         <v>528</v>
       </c>
       <c r="AJ145" s="40" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v/>
       </c>
     </row>
@@ -25096,7 +25133,7 @@
         <v>529</v>
       </c>
       <c r="AJ146" s="40" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v/>
       </c>
     </row>
@@ -25125,7 +25162,7 @@
         <v>530</v>
       </c>
       <c r="AJ147" s="40" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v/>
       </c>
     </row>
@@ -25149,7 +25186,7 @@
         <v>531</v>
       </c>
       <c r="AJ148" s="40" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v/>
       </c>
     </row>
@@ -25173,7 +25210,7 @@
         <v>533</v>
       </c>
       <c r="AJ149" s="40" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v/>
       </c>
     </row>
@@ -25195,7 +25232,7 @@
         <v>534</v>
       </c>
       <c r="AJ150" s="40" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v/>
       </c>
     </row>
@@ -25217,7 +25254,7 @@
         <v>536</v>
       </c>
       <c r="AJ151" s="40" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v/>
       </c>
     </row>
@@ -25234,7 +25271,7 @@
         <v>538</v>
       </c>
       <c r="AJ152" s="40" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v/>
       </c>
     </row>
@@ -25251,7 +25288,7 @@
         <v>540</v>
       </c>
       <c r="AJ153" s="40" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v/>
       </c>
     </row>
@@ -25268,7 +25305,7 @@
         <v>541</v>
       </c>
       <c r="AJ154" s="40" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v/>
       </c>
     </row>
@@ -25285,7 +25322,7 @@
         <v>1041</v>
       </c>
       <c r="AJ155" s="40" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v/>
       </c>
     </row>
@@ -25305,7 +25342,7 @@
         <v>1042</v>
       </c>
       <c r="AJ156" s="40" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v/>
       </c>
     </row>
@@ -25338,7 +25375,7 @@
         <v>1043</v>
       </c>
       <c r="AJ157" s="40" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v/>
       </c>
     </row>
@@ -25373,7 +25410,7 @@
         <v>1044</v>
       </c>
       <c r="AJ158" s="40" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v/>
       </c>
     </row>
@@ -25408,7 +25445,7 @@
         <v>1045</v>
       </c>
       <c r="AJ159" s="40" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v/>
       </c>
     </row>
@@ -25439,7 +25476,7 @@
         <v>1046</v>
       </c>
       <c r="AJ160" s="40" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v/>
       </c>
     </row>
@@ -25470,7 +25507,7 @@
         <v>1047</v>
       </c>
       <c r="AJ161" s="40" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v/>
       </c>
     </row>
@@ -25494,7 +25531,7 @@
         <v>1048</v>
       </c>
       <c r="AJ162" s="40" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v/>
       </c>
     </row>
@@ -25518,7 +25555,7 @@
         <v>1049</v>
       </c>
       <c r="AJ163" s="40" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v/>
       </c>
     </row>
@@ -25542,7 +25579,7 @@
         <v>1050</v>
       </c>
       <c r="AJ164" s="40" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v/>
       </c>
     </row>
@@ -25566,7 +25603,7 @@
         <v>1051</v>
       </c>
       <c r="AJ165" s="40" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v/>
       </c>
     </row>
@@ -25586,7 +25623,7 @@
         <v>1052</v>
       </c>
       <c r="AJ166" s="40" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v/>
       </c>
     </row>
@@ -25619,7 +25656,7 @@
         <v>1053</v>
       </c>
       <c r="AJ167" s="40" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v/>
       </c>
     </row>
@@ -25653,7 +25690,7 @@
         <v>1054</v>
       </c>
       <c r="AJ168" s="40" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v/>
       </c>
     </row>
@@ -25688,7 +25725,7 @@
         <v>1055</v>
       </c>
       <c r="AJ169" s="40" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v/>
       </c>
     </row>
@@ -25712,7 +25749,7 @@
         <v>1056</v>
       </c>
       <c r="AJ170" s="40" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v/>
       </c>
     </row>
@@ -25736,7 +25773,7 @@
         <v>1057</v>
       </c>
       <c r="AJ171" s="40" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v/>
       </c>
     </row>
@@ -25760,7 +25797,7 @@
         <v>1058</v>
       </c>
       <c r="AJ172" s="40" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v/>
       </c>
     </row>
@@ -25784,7 +25821,7 @@
         <v>1059</v>
       </c>
       <c r="AJ173" s="40" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v/>
       </c>
     </row>
@@ -25801,7 +25838,7 @@
         <v>1060</v>
       </c>
       <c r="AJ174" s="40" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v/>
       </c>
     </row>
@@ -25818,7 +25855,7 @@
         <v>1061</v>
       </c>
       <c r="AJ175" s="40" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v/>
       </c>
     </row>
@@ -25835,7 +25872,7 @@
         <v>1062</v>
       </c>
       <c r="AJ176" s="40" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v/>
       </c>
     </row>
@@ -25855,7 +25892,7 @@
         <v>544</v>
       </c>
       <c r="AJ177" s="40" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v/>
       </c>
     </row>
@@ -25888,7 +25925,7 @@
         <v>1063</v>
       </c>
       <c r="AJ178" s="40" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v/>
       </c>
     </row>
@@ -25920,7 +25957,7 @@
         <v>1064</v>
       </c>
       <c r="AJ179" s="40" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v/>
       </c>
     </row>
@@ -25952,7 +25989,7 @@
         <v>1065</v>
       </c>
       <c r="AJ180" s="40" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v/>
       </c>
     </row>
@@ -25980,7 +26017,7 @@
         <v>1066</v>
       </c>
       <c r="AJ181" s="40" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v/>
       </c>
     </row>
@@ -26002,7 +26039,7 @@
         <v>1067</v>
       </c>
       <c r="AJ182" s="40" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v/>
       </c>
     </row>
@@ -26030,7 +26067,7 @@
         <v>1068</v>
       </c>
       <c r="AJ183" s="40" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v/>
       </c>
     </row>
@@ -26051,7 +26088,7 @@
         <v>1069</v>
       </c>
       <c r="AJ184" s="40" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v/>
       </c>
     </row>
@@ -26072,7 +26109,7 @@
         <v>545</v>
       </c>
       <c r="AJ185" s="40" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v/>
       </c>
     </row>
@@ -26093,7 +26130,7 @@
         <v>546</v>
       </c>
       <c r="AJ186" s="40" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v/>
       </c>
     </row>
@@ -26114,7 +26151,7 @@
         <v>548</v>
       </c>
       <c r="AJ187" s="40" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v/>
       </c>
     </row>
@@ -26135,7 +26172,7 @@
         <v>549</v>
       </c>
       <c r="AJ188" s="40" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v/>
       </c>
     </row>
@@ -26156,7 +26193,7 @@
         <v>551</v>
       </c>
       <c r="AJ189" s="40" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v/>
       </c>
     </row>
@@ -26177,7 +26214,7 @@
         <v>553</v>
       </c>
       <c r="AJ190" s="40" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v/>
       </c>
     </row>
@@ -26191,7 +26228,7 @@
         <v>555</v>
       </c>
       <c r="AJ191" s="40" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v/>
       </c>
     </row>
@@ -26205,7 +26242,7 @@
         <v>556</v>
       </c>
       <c r="AJ192" s="40" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v/>
       </c>
     </row>
@@ -26219,7 +26256,7 @@
         <v>1116</v>
       </c>
       <c r="AJ193" s="40" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v/>
       </c>
     </row>
@@ -26236,7 +26273,7 @@
         <v>1117</v>
       </c>
       <c r="AJ194" s="40" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v/>
       </c>
     </row>
@@ -26266,7 +26303,7 @@
         <v>1118</v>
       </c>
       <c r="AJ195" s="40" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v/>
       </c>
     </row>
@@ -26298,7 +26335,7 @@
         <v>1119</v>
       </c>
       <c r="AJ196" s="40" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v/>
       </c>
     </row>
@@ -26327,7 +26364,7 @@
         <v>1120</v>
       </c>
       <c r="AJ197" s="40" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v/>
       </c>
     </row>
@@ -26355,7 +26392,7 @@
         <v>1121</v>
       </c>
       <c r="AJ198" s="40" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v/>
       </c>
     </row>
@@ -26383,7 +26420,7 @@
         <v>1122</v>
       </c>
       <c r="AJ199" s="40" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v/>
       </c>
     </row>
@@ -26404,7 +26441,7 @@
         <v>1123</v>
       </c>
       <c r="AJ200" s="40" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v/>
       </c>
     </row>
@@ -26425,7 +26462,7 @@
         <v>1124</v>
       </c>
       <c r="AJ201" s="40" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v/>
       </c>
     </row>
@@ -27217,7 +27254,7 @@
   </sheetPr>
   <dimension ref="A2:AC91"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="B22" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
@@ -27249,26 +27286,26 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:8" ht="30">
-      <c r="C2" s="575" t="s">
+      <c r="C2" s="590" t="s">
         <v>944</v>
       </c>
-      <c r="D2" s="576"/>
+      <c r="D2" s="591"/>
       <c r="E2" s="299" t="s">
         <v>945</v>
       </c>
-      <c r="F2" s="583" t="s">
+      <c r="F2" s="597" t="s">
         <v>976</v>
       </c>
-      <c r="G2" s="584"/>
+      <c r="G2" s="598"/>
       <c r="H2" s="318" t="s">
         <v>970</v>
       </c>
     </row>
     <row r="3" spans="3:8">
-      <c r="C3" s="573" t="s">
+      <c r="C3" s="576" t="s">
         <v>975</v>
       </c>
-      <c r="D3" s="574"/>
+      <c r="D3" s="577"/>
       <c r="E3" s="378" t="e">
         <f>Inputs!AD10</f>
         <v>#N/A</v>
@@ -27296,10 +27333,10 @@
       </c>
     </row>
     <row r="5" spans="3:8" hidden="1" outlineLevel="1">
-      <c r="C5" s="573" t="s">
+      <c r="C5" s="576" t="s">
         <v>956</v>
       </c>
-      <c r="D5" s="574"/>
+      <c r="D5" s="577"/>
       <c r="E5" s="379" t="e">
         <f>VLOOKUP(E3,'Conditions (june 2020)'!B:AK,36,FALSE)</f>
         <v>#N/A</v>
@@ -27312,10 +27349,10 @@
       </c>
     </row>
     <row r="6" spans="3:8" hidden="1" outlineLevel="1">
-      <c r="C6" s="573" t="s">
+      <c r="C6" s="576" t="s">
         <v>761</v>
       </c>
-      <c r="D6" s="574"/>
+      <c r="D6" s="577"/>
       <c r="E6" s="379" t="e">
         <f>VLOOKUP(E3,'Conditions (june 2020)'!B:AK,35,FALSE)</f>
         <v>#N/A</v>
@@ -27325,10 +27362,10 @@
       <c r="H6" s="310"/>
     </row>
     <row r="7" spans="3:8" hidden="1" outlineLevel="1">
-      <c r="C7" s="573" t="s">
+      <c r="C7" s="576" t="s">
         <v>967</v>
       </c>
-      <c r="D7" s="574"/>
+      <c r="D7" s="577"/>
       <c r="E7" s="379" t="e">
         <f>VLOOKUP(E3,'Conditions (june 2020)'!B:AK,34,FALSE)</f>
         <v>#N/A</v>
@@ -27338,73 +27375,73 @@
       <c r="H7" s="310"/>
     </row>
     <row r="8" spans="3:8" s="381" customFormat="1" collapsed="1">
-      <c r="C8" s="577" t="s">
+      <c r="C8" s="592" t="s">
         <v>923</v>
       </c>
-      <c r="D8" s="578"/>
+      <c r="D8" s="593"/>
       <c r="E8" s="380" t="str">
         <f>Inputs!H28</f>
         <v/>
       </c>
-      <c r="F8" s="579">
+      <c r="F8" s="594">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="G8" s="580"/>
+      <c r="G8" s="579"/>
       <c r="H8" s="310">
         <f>IF(E8&gt;0,0,1)</f>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="3:8">
-      <c r="C9" s="589"/>
-      <c r="D9" s="586"/>
+      <c r="C9" s="580"/>
+      <c r="D9" s="581"/>
       <c r="E9" s="382"/>
       <c r="F9" s="272"/>
       <c r="G9" s="273"/>
       <c r="H9" s="310"/>
     </row>
     <row r="10" spans="3:8" ht="16.5" customHeight="1">
-      <c r="C10" s="581" t="s">
+      <c r="C10" s="595" t="s">
         <v>1005</v>
       </c>
-      <c r="D10" s="582"/>
+      <c r="D10" s="596"/>
       <c r="E10" s="380">
         <f>Inputs!H11</f>
         <v>0</v>
       </c>
-      <c r="F10" s="585">
-        <v>0</v>
-      </c>
-      <c r="G10" s="586"/>
+      <c r="F10" s="599">
+        <v>0</v>
+      </c>
+      <c r="G10" s="581"/>
       <c r="H10" s="310">
         <f>IF(E10&gt;F10,1,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="3:8">
-      <c r="C11" s="573" t="s">
+      <c r="C11" s="576" t="s">
         <v>924</v>
       </c>
-      <c r="D11" s="574"/>
+      <c r="D11" s="577"/>
       <c r="E11" s="431">
         <f>Inputs!H12</f>
         <v>0</v>
       </c>
-      <c r="F11" s="590">
+      <c r="F11" s="582">
         <f>IFERROR(VLOOKUP(E3,'Conditions (june 2020)'!B:H,7,FALSE)*100,0)</f>
         <v>0</v>
       </c>
-      <c r="G11" s="591"/>
+      <c r="G11" s="583"/>
       <c r="H11" s="310">
         <f>IF(E11&gt;F11,1,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="3:8">
-      <c r="C12" s="573" t="s">
+      <c r="C12" s="576" t="s">
         <v>925</v>
       </c>
-      <c r="D12" s="574"/>
+      <c r="D12" s="577"/>
       <c r="E12" s="383">
         <f ca="1">YEAR(TODAY())-Inputs!C11</f>
         <v>2021</v>
@@ -27414,64 +27451,64 @@
       <c r="H12" s="310"/>
     </row>
     <row r="13" spans="3:8">
-      <c r="C13" s="573" t="s">
+      <c r="C13" s="576" t="s">
         <v>926</v>
       </c>
-      <c r="D13" s="574"/>
+      <c r="D13" s="577"/>
       <c r="E13" s="383">
         <f>Inputs!H25</f>
         <v>0</v>
       </c>
-      <c r="F13" s="588">
+      <c r="F13" s="578">
         <v>3</v>
       </c>
-      <c r="G13" s="580"/>
+      <c r="G13" s="579"/>
       <c r="H13" s="310">
         <f>IF(E13&gt;=F13,0,1)</f>
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="3:8">
-      <c r="C14" s="573" t="s">
+      <c r="C14" s="576" t="s">
         <v>1007</v>
       </c>
-      <c r="D14" s="574"/>
+      <c r="D14" s="577"/>
       <c r="E14" s="383">
         <f>Inputs!H9</f>
         <v>0</v>
       </c>
-      <c r="F14" s="592" t="s">
+      <c r="F14" s="584" t="s">
         <v>58</v>
       </c>
-      <c r="G14" s="586"/>
+      <c r="G14" s="581"/>
       <c r="H14" s="310">
         <f>IF(E14=F14,0,1)</f>
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="3:8">
-      <c r="C15" s="573" t="s">
+      <c r="C15" s="576" t="s">
         <v>927</v>
       </c>
-      <c r="D15" s="574"/>
+      <c r="D15" s="577"/>
       <c r="E15" s="383" t="str">
         <f>Inputs!H26</f>
         <v>Yes</v>
       </c>
-      <c r="F15" s="592" t="s">
+      <c r="F15" s="584" t="s">
         <v>90</v>
       </c>
-      <c r="G15" s="586"/>
+      <c r="G15" s="581"/>
       <c r="H15" s="310">
         <f>IF(E15=F15,0,1)</f>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="3:8">
-      <c r="C16" s="573" t="s">
+      <c r="C16" s="576" t="s">
         <v>1006</v>
       </c>
-      <c r="D16" s="574"/>
+      <c r="D16" s="577"/>
       <c r="E16" s="384"/>
       <c r="F16" s="323">
         <v>0.1</v>
@@ -27480,18 +27517,18 @@
       <c r="H16" s="310"/>
     </row>
     <row r="17" spans="3:27">
-      <c r="C17" s="593" t="s">
+      <c r="C17" s="585" t="s">
         <v>928</v>
       </c>
-      <c r="D17" s="594"/>
+      <c r="D17" s="586"/>
       <c r="E17" s="385">
         <f>Inputs!AD19</f>
         <v>0</v>
       </c>
-      <c r="F17" s="570">
+      <c r="F17" s="587">
         <v>2000000</v>
       </c>
-      <c r="G17" s="571"/>
+      <c r="G17" s="588"/>
       <c r="H17" s="310">
         <f>IF(E17&lt;=F17,0,1)</f>
         <v>0</v>
@@ -27578,13 +27615,13 @@
       </c>
     </row>
     <row r="23" spans="3:27" ht="20.399999999999999">
-      <c r="C23" s="572" t="s">
+      <c r="C23" s="589" t="s">
         <v>930</v>
       </c>
-      <c r="D23" s="572"/>
-      <c r="E23" s="572"/>
-      <c r="F23" s="572"/>
-      <c r="G23" s="572"/>
+      <c r="D23" s="589"/>
+      <c r="E23" s="589"/>
+      <c r="F23" s="589"/>
+      <c r="G23" s="589"/>
       <c r="H23" s="371"/>
     </row>
     <row r="24" spans="3:27" ht="16.8">
@@ -28427,11 +28464,11 @@
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I47" s="587" t="s">
+      <c r="I47" s="575" t="s">
         <v>968</v>
       </c>
-      <c r="J47" s="587"/>
-      <c r="K47" s="587"/>
+      <c r="J47" s="575"/>
+      <c r="K47" s="575"/>
       <c r="M47" s="410" t="s">
         <v>969</v>
       </c>
@@ -29391,6 +29428,15 @@
   </sheetData>
   <sheetProtection password="93C0" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="25">
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="F10:G10"/>
     <mergeCell ref="I47:K47"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C5:D5"/>
@@ -29407,15 +29453,6 @@
     <mergeCell ref="C16:D16"/>
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="F14:G14"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="F10:G10"/>
   </mergeCells>
   <conditionalFormatting sqref="F8:H8 H9:H11 H13:H18 H20 H4">
     <cfRule type="containsText" dxfId="65" priority="195" operator="containsText" text="Le % de Chiffre d'Affaires Électricien indiqué est inférieur à 90%">
@@ -40012,20 +40049,20 @@
       <c r="B4" s="440" t="s">
         <v>700</v>
       </c>
-      <c r="C4" s="599" t="s">
+      <c r="C4" s="604" t="s">
         <v>701</v>
       </c>
-      <c r="D4" s="600"/>
+      <c r="D4" s="605"/>
       <c r="E4" s="441"/>
-      <c r="H4" s="601" t="s">
+      <c r="H4" s="606" t="s">
         <v>702</v>
       </c>
-      <c r="I4" s="602"/>
-      <c r="J4" s="603"/>
-      <c r="M4" s="604" t="s">
+      <c r="I4" s="607"/>
+      <c r="J4" s="608"/>
+      <c r="M4" s="609" t="s">
         <v>703</v>
       </c>
-      <c r="N4" s="605"/>
+      <c r="N4" s="610"/>
     </row>
     <row r="5" spans="1:14" ht="28.8">
       <c r="A5" s="442"/>
@@ -40046,8 +40083,8 @@
       <c r="J5" s="448" t="s">
         <v>708</v>
       </c>
-      <c r="M5" s="606"/>
-      <c r="N5" s="607"/>
+      <c r="M5" s="611"/>
+      <c r="N5" s="612"/>
     </row>
     <row r="6" spans="1:14" ht="30" customHeight="1">
       <c r="A6" s="449" t="s">
@@ -40056,24 +40093,24 @@
       <c r="B6" s="450" t="s">
         <v>710</v>
       </c>
-      <c r="C6" s="610" t="s">
+      <c r="C6" s="615" t="s">
         <v>711</v>
       </c>
-      <c r="D6" s="611"/>
+      <c r="D6" s="616"/>
       <c r="E6" s="451" t="s">
         <v>712</v>
       </c>
       <c r="H6" s="452" t="s">
         <v>713</v>
       </c>
-      <c r="I6" s="612" t="s">
+      <c r="I6" s="617" t="s">
         <v>714</v>
       </c>
       <c r="J6" s="452">
         <v>0</v>
       </c>
-      <c r="M6" s="606"/>
-      <c r="N6" s="607"/>
+      <c r="M6" s="611"/>
+      <c r="N6" s="612"/>
     </row>
     <row r="7" spans="1:14">
       <c r="A7" s="453" t="s">
@@ -40095,12 +40132,12 @@
       <c r="H7" s="457" t="s">
         <v>717</v>
       </c>
-      <c r="I7" s="613"/>
+      <c r="I7" s="618"/>
       <c r="J7" s="457">
         <v>0.2</v>
       </c>
-      <c r="M7" s="606"/>
-      <c r="N7" s="607"/>
+      <c r="M7" s="611"/>
+      <c r="N7" s="612"/>
     </row>
     <row r="8" spans="1:14" ht="24" customHeight="1">
       <c r="A8" s="458" t="s">
@@ -40122,14 +40159,14 @@
       <c r="H8" s="462" t="s">
         <v>719</v>
       </c>
-      <c r="I8" s="614" t="s">
+      <c r="I8" s="619" t="s">
         <v>720</v>
       </c>
       <c r="J8" s="462">
         <v>0.35</v>
       </c>
-      <c r="M8" s="606"/>
-      <c r="N8" s="607"/>
+      <c r="M8" s="611"/>
+      <c r="N8" s="612"/>
     </row>
     <row r="9" spans="1:14" ht="24.75" customHeight="1">
       <c r="A9" s="458" t="s">
@@ -40151,12 +40188,12 @@
       <c r="H9" s="457" t="s">
         <v>722</v>
       </c>
-      <c r="I9" s="613"/>
+      <c r="I9" s="618"/>
       <c r="J9" s="457">
         <v>0.5</v>
       </c>
-      <c r="M9" s="608"/>
-      <c r="N9" s="609"/>
+      <c r="M9" s="613"/>
+      <c r="N9" s="614"/>
     </row>
     <row r="10" spans="1:14">
       <c r="A10" s="463" t="s">
@@ -40255,13 +40292,13 @@
       <c r="E15" s="480"/>
       <c r="F15" s="481"/>
       <c r="G15" s="482"/>
-      <c r="H15" s="615"/>
-      <c r="I15" s="615"/>
-      <c r="J15" s="615"/>
-      <c r="K15" s="615"/>
-      <c r="L15" s="615"/>
-      <c r="M15" s="615"/>
-      <c r="N15" s="616"/>
+      <c r="H15" s="620"/>
+      <c r="I15" s="620"/>
+      <c r="J15" s="620"/>
+      <c r="K15" s="620"/>
+      <c r="L15" s="620"/>
+      <c r="M15" s="620"/>
+      <c r="N15" s="621"/>
     </row>
     <row r="16" spans="1:14" s="483" customFormat="1" outlineLevel="1">
       <c r="B16" s="484"/>
@@ -40320,10 +40357,10 @@
       <c r="E19" s="497">
         <v>4</v>
       </c>
-      <c r="F19" s="595" t="s">
+      <c r="F19" s="600" t="s">
         <v>732</v>
       </c>
-      <c r="G19" s="596"/>
+      <c r="G19" s="601"/>
       <c r="H19" s="495">
         <v>1</v>
       </c>
@@ -40336,10 +40373,10 @@
       <c r="K19" s="497">
         <v>4</v>
       </c>
-      <c r="M19" s="597" t="s">
+      <c r="M19" s="602" t="s">
         <v>732</v>
       </c>
-      <c r="N19" s="598"/>
+      <c r="N19" s="603"/>
     </row>
     <row r="20" spans="1:14" ht="31.5" customHeight="1">
       <c r="B20" s="498" t="str">

</xml_diff>